<commit_message>
tabela correlacao com qps
</commit_message>
<xml_diff>
--- a/Tabela_Correlacao.xlsx
+++ b/Tabela_Correlacao.xlsx
@@ -663,35 +663,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:Z45" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:Z45" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:Z45"/>
+  <sortState ref="A2:Z45">
+    <sortCondition ref="A1:A45"/>
+  </sortState>
   <tableColumns count="26">
-    <tableColumn id="1" name="Curso" dataDxfId="27"/>
-    <tableColumn id="2" name="nota_fg x i7_qtde_familiares_em_casa" dataDxfId="26"/>
-    <tableColumn id="3" name="nota_fg x renda" dataDxfId="25"/>
-    <tableColumn id="4" name="nota_fg X situacao_trabalho" dataDxfId="24"/>
-    <tableColumn id="5" name="nota_fg x livros" dataDxfId="23"/>
-    <tableColumn id="6" name="nota_fg  x horas estudo semana" dataDxfId="22"/>
-    <tableColumn id="7" name="nota_CE x i7_qtde_familiares_em_casa" dataDxfId="21"/>
-    <tableColumn id="8" name="nota_CE x renda" dataDxfId="20"/>
-    <tableColumn id="9" name="nota_CE X situacao_trabalho" dataDxfId="19"/>
-    <tableColumn id="10" name="nota_CE x livros" dataDxfId="18"/>
-    <tableColumn id="11" name="nota_CE  x horas estudo semana" dataDxfId="17"/>
-    <tableColumn id="12" name="nota_GER x i7_qtde_familiares_em_casa" dataDxfId="16"/>
-    <tableColumn id="13" name="nota_GER x renda" dataDxfId="15"/>
-    <tableColumn id="14" name="nota_GER X situacao_trabalho" dataDxfId="14"/>
-    <tableColumn id="15" name="nota_GER x livros" dataDxfId="13"/>
-    <tableColumn id="16" name="nota_GER  x horas estudo semana" dataDxfId="12"/>
-    <tableColumn id="17" name="qtd_familiares x renda" dataDxfId="11"/>
-    <tableColumn id="18" name="qtd_familiares x situacao_trabalho" dataDxfId="10"/>
-    <tableColumn id="19" name="qtd_familiares x livros" dataDxfId="9"/>
-    <tableColumn id="20" name="qtd_familiares x horas_estudo" dataDxfId="8"/>
-    <tableColumn id="21" name="renda x situacao trabalho" dataDxfId="7"/>
-    <tableColumn id="22" name="renda x livros" dataDxfId="6"/>
-    <tableColumn id="23" name="renda x  horas_estudo" dataDxfId="5"/>
-    <tableColumn id="24" name="situacao_trabalho x livros" dataDxfId="4"/>
-    <tableColumn id="25" name="situacao_trabalho x horas_estudo" dataDxfId="3"/>
-    <tableColumn id="26" name="livros x horas_estudo" dataDxfId="2"/>
+    <tableColumn id="1" name="Curso" dataDxfId="25"/>
+    <tableColumn id="2" name="nota_fg x i7_qtde_familiares_em_casa" dataDxfId="24"/>
+    <tableColumn id="3" name="nota_fg x renda" dataDxfId="23"/>
+    <tableColumn id="4" name="nota_fg X situacao_trabalho" dataDxfId="22"/>
+    <tableColumn id="5" name="nota_fg x livros" dataDxfId="21"/>
+    <tableColumn id="6" name="nota_fg  x horas estudo semana" dataDxfId="20"/>
+    <tableColumn id="7" name="nota_CE x i7_qtde_familiares_em_casa" dataDxfId="19"/>
+    <tableColumn id="8" name="nota_CE x renda" dataDxfId="18"/>
+    <tableColumn id="9" name="nota_CE X situacao_trabalho" dataDxfId="17"/>
+    <tableColumn id="10" name="nota_CE x livros" dataDxfId="16"/>
+    <tableColumn id="11" name="nota_CE  x horas estudo semana" dataDxfId="15"/>
+    <tableColumn id="12" name="nota_GER x i7_qtde_familiares_em_casa" dataDxfId="14"/>
+    <tableColumn id="13" name="nota_GER x renda" dataDxfId="13"/>
+    <tableColumn id="14" name="nota_GER X situacao_trabalho" dataDxfId="12"/>
+    <tableColumn id="15" name="nota_GER x livros" dataDxfId="11"/>
+    <tableColumn id="16" name="nota_GER  x horas estudo semana" dataDxfId="10"/>
+    <tableColumn id="17" name="qtd_familiares x renda" dataDxfId="9"/>
+    <tableColumn id="18" name="qtd_familiares x situacao_trabalho" dataDxfId="8"/>
+    <tableColumn id="19" name="qtd_familiares x livros" dataDxfId="7"/>
+    <tableColumn id="20" name="qtd_familiares x horas_estudo" dataDxfId="6"/>
+    <tableColumn id="21" name="renda x situacao trabalho" dataDxfId="5"/>
+    <tableColumn id="22" name="renda x livros" dataDxfId="4"/>
+    <tableColumn id="23" name="renda x  horas_estudo" dataDxfId="3"/>
+    <tableColumn id="24" name="situacao_trabalho x livros" dataDxfId="2"/>
+    <tableColumn id="25" name="situacao_trabalho x horas_estudo" dataDxfId="1"/>
+    <tableColumn id="26" name="livros x horas_estudo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -963,7 +966,7 @@
   <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1078,3522 +1081,3522 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
-        <v>1.7690629764599999E-3</v>
+        <v>-7.4749637834899997E-3</v>
       </c>
       <c r="C2" s="1">
-        <v>5.1348427399600001E-2</v>
+        <v>7.3570315087599994E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>2.5125257576199999E-2</v>
+        <v>-5.8475676702199997E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>4.7752578873299999E-2</v>
+        <v>4.9425962541599998E-2</v>
       </c>
       <c r="F2" s="1">
-        <v>7.36955385543E-2</v>
+        <v>7.9185314700099999E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>-5.5882109569099997E-3</v>
+        <v>-2.45873549697E-2</v>
       </c>
       <c r="H2" s="1">
-        <v>9.6245854573600007E-2</v>
+        <v>7.0131988160800005E-2</v>
       </c>
       <c r="I2" s="1">
-        <v>4.5379994655500001E-2</v>
+        <v>-8.3689787710300001E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>6.4317832916699999E-2</v>
+        <v>7.2418768250699997E-2</v>
       </c>
       <c r="K2" s="1">
-        <v>0.107470280694</v>
+        <v>0.139869360222</v>
       </c>
       <c r="L2" s="1">
-        <v>-4.0366512223999999E-3</v>
+        <v>-2.2061699877000001E-2</v>
       </c>
       <c r="M2" s="1">
-        <v>9.4908058614099997E-2</v>
+        <v>8.0656417325499996E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>4.5051907139499997E-2</v>
+        <v>-8.6288976945500001E-2</v>
       </c>
       <c r="O2" s="1">
-        <v>6.7630911737000005E-2</v>
+        <v>7.4227044141899998E-2</v>
       </c>
       <c r="P2" s="1">
-        <v>0.111105518518</v>
+        <v>0.13787050108099999</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.31949992458900001</v>
+        <v>0.22861538844400001</v>
       </c>
       <c r="R2" s="1">
-        <v>0.44303051447500003</v>
+        <v>0.13580709846700001</v>
       </c>
       <c r="S2" s="1">
-        <v>0.34813304121100003</v>
+        <v>0.224119019186</v>
       </c>
       <c r="T2" s="1">
-        <v>0.31137035045400002</v>
+        <v>0.221594611</v>
       </c>
       <c r="U2" s="1">
-        <v>0.394806687928</v>
+        <v>2.7424427285999999E-2</v>
       </c>
       <c r="V2" s="1">
-        <v>0.203568968578</v>
+        <v>0.125851671996</v>
       </c>
       <c r="W2" s="1">
-        <v>0.21532745219900001</v>
+        <v>0.17979040218799999</v>
       </c>
       <c r="X2" s="1">
-        <v>0.37168828921699998</v>
+        <v>0.110407354428</v>
       </c>
       <c r="Y2" s="1">
-        <v>0.34070829022400001</v>
+        <v>3.7936468679099999E-2</v>
       </c>
       <c r="Z2" s="1">
-        <v>0.473039622351</v>
+        <v>0.325753323426</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
-        <v>-4.9356262117300001E-2</v>
+        <v>-6.0943001463600002E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>7.3860828859200006E-2</v>
+        <v>0.17763838615999999</v>
       </c>
       <c r="D3" s="1">
-        <v>2.9052145772599999E-2</v>
+        <v>-2.05294289244E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>9.2867531534299996E-2</v>
+        <v>5.6290141288299997E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>6.4420701104699996E-2</v>
+        <v>7.9347502315100002E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>-2.4376765478399998E-2</v>
+        <v>-8.7964434996600005E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>0.121442021668</v>
+        <v>0.20990955924999999</v>
       </c>
       <c r="I3" s="1">
-        <v>8.3759628983599996E-2</v>
+        <v>-9.0183131109100007E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>8.1917605886699996E-2</v>
+        <v>9.8603631403099995E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>0.121121554258</v>
+        <v>0.11211687144099999</v>
       </c>
       <c r="L3" s="1">
-        <v>-3.6884993195999999E-2</v>
+        <v>-8.9531984609900001E-2</v>
       </c>
       <c r="M3" s="1">
-        <v>0.12536203219100001</v>
+        <v>0.22287165274099999</v>
       </c>
       <c r="N3" s="1">
-        <v>7.9036392638200004E-2</v>
+        <v>-7.9696724460700002E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>9.9215506699999997E-2</v>
+        <v>9.6855214829400002E-2</v>
       </c>
       <c r="P3" s="1">
-        <v>0.121935047724</v>
+        <v>0.114587301192</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.372122777628</v>
+        <v>0.30486368692799998</v>
       </c>
       <c r="R3" s="1">
-        <v>0.47004949580900002</v>
+        <v>0.34977602885699999</v>
       </c>
       <c r="S3" s="1">
-        <v>0.42363550668</v>
+        <v>0.44582551193499997</v>
       </c>
       <c r="T3" s="1">
-        <v>0.40569293974300003</v>
+        <v>0.37714996334200002</v>
       </c>
       <c r="U3" s="1">
-        <v>0.39750788179000002</v>
+        <v>0.27836945324500001</v>
       </c>
       <c r="V3" s="1">
-        <v>0.24354709608700001</v>
+        <v>0.26461320972800001</v>
       </c>
       <c r="W3" s="1">
-        <v>0.240934412376</v>
+        <v>0.27902810883500001</v>
       </c>
       <c r="X3" s="1">
-        <v>0.38180046187299999</v>
+        <v>0.328096302723</v>
       </c>
       <c r="Y3" s="1">
-        <v>0.37819101847199998</v>
+        <v>0.28577752312499999</v>
       </c>
       <c r="Z3" s="1">
-        <v>0.55175710154099999</v>
+        <v>0.55781539900999999</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1">
-        <v>-6.0443076936199998E-2</v>
+        <v>-3.8345240647599997E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.13447018481799999</v>
+        <v>6.9444446596800005E-2</v>
       </c>
       <c r="D4" s="1">
-        <v>3.4876068761400002E-2</v>
+        <v>-6.9741999434299998E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>6.2718460290299996E-2</v>
+        <v>5.2320401696499999E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>8.4307893024599997E-2</v>
+        <v>0.105186273025</v>
       </c>
       <c r="G4" s="1">
-        <v>-9.3120268845800006E-2</v>
+        <v>-7.1488258945300004E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>0.21028877804000001</v>
+        <v>0.153980502953</v>
       </c>
       <c r="I4" s="1">
-        <v>-8.6834126329499994E-2</v>
+        <v>-0.20416884763900001</v>
       </c>
       <c r="J4" s="1">
-        <v>0.117960776074</v>
+        <v>3.0877228387100001E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>0.15854403560899999</v>
+        <v>0.18263973725999999</v>
       </c>
       <c r="L4" s="1">
-        <v>-9.3913483912099999E-2</v>
+        <v>-7.1856493866599994E-2</v>
       </c>
       <c r="M4" s="1">
-        <v>0.21147128200099999</v>
+        <v>0.15049238186200001</v>
       </c>
       <c r="N4" s="1">
-        <v>-6.0982612889600003E-2</v>
+        <v>-0.19234149195899999</v>
       </c>
       <c r="O4" s="1">
-        <v>0.11491277131700001</v>
+        <v>4.2648868553399999E-2</v>
       </c>
       <c r="P4" s="1">
-        <v>0.15444407948399999</v>
+        <v>0.18593148695699999</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.22651795506799999</v>
+        <v>0.24794692906599999</v>
       </c>
       <c r="R4" s="1">
-        <v>0.29090942033799999</v>
+        <v>0.233259913111</v>
       </c>
       <c r="S4" s="1">
-        <v>0.434274155188</v>
+        <v>0.26510829057500002</v>
       </c>
       <c r="T4" s="1">
-        <v>0.35069108585100001</v>
+        <v>0.248704084873</v>
       </c>
       <c r="U4" s="1">
-        <v>0.233008844902</v>
+        <v>0.19475649623999999</v>
       </c>
       <c r="V4" s="1">
-        <v>0.24755359811700001</v>
+        <v>0.15183802320500001</v>
       </c>
       <c r="W4" s="1">
-        <v>0.21563629644499999</v>
+        <v>0.143249106509</v>
       </c>
       <c r="X4" s="1">
-        <v>0.27600039900399997</v>
+        <v>0.17348168556499999</v>
       </c>
       <c r="Y4" s="1">
-        <v>0.21248613290599999</v>
+        <v>5.65548299709E-2</v>
       </c>
       <c r="Z4" s="1">
-        <v>0.55733293480000001</v>
+        <v>0.39486474678299999</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1">
-        <v>-3.1189675450800002E-2</v>
+        <v>-8.6846705604399999E-2</v>
       </c>
       <c r="C5" s="1">
-        <v>4.86474404919E-2</v>
+        <v>8.9134465684999997E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>-2.5296086075100001E-2</v>
+        <v>4.25647507299E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>9.2075988445800006E-2</v>
+        <v>-2.3613114355399999E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>5.3935724810800001E-2</v>
+        <v>6.7713552056899995E-2</v>
       </c>
       <c r="G5" s="1">
-        <v>-8.2157628113399994E-2</v>
+        <v>-0.109236455607</v>
       </c>
       <c r="H5" s="1">
-        <v>0.152722669374</v>
+        <v>0.17214113169100001</v>
       </c>
       <c r="I5" s="1">
-        <v>4.34554878329E-2</v>
+        <v>3.17895646638E-2</v>
       </c>
       <c r="J5" s="1">
-        <v>2.3217635633599999E-2</v>
+        <v>-2.80541963615E-2</v>
       </c>
       <c r="K5" s="1">
-        <v>6.5830212838800001E-2</v>
+        <v>0.122676288038</v>
       </c>
       <c r="L5" s="1">
-        <v>-7.9110748520499999E-2</v>
+        <v>-0.114933318366</v>
       </c>
       <c r="M5" s="1">
-        <v>0.144250769433</v>
+        <v>0.16709433291199999</v>
       </c>
       <c r="N5" s="1">
-        <v>2.9309367954899999E-2</v>
+        <v>3.8543227091100002E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>4.7280732657299998E-2</v>
+        <v>-2.9912703459899999E-2</v>
       </c>
       <c r="P5" s="1">
-        <v>7.1997185376900003E-2</v>
+        <v>0.12030488244900001</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.38642427277500002</v>
+        <v>0.20843667672300001</v>
       </c>
       <c r="R5" s="1">
-        <v>0.47355002546800001</v>
+        <v>0.32185713847199998</v>
       </c>
       <c r="S5" s="1">
-        <v>0.38699418011600001</v>
+        <v>0.38309032618599997</v>
       </c>
       <c r="T5" s="1">
-        <v>0.35952585422900002</v>
+        <v>0.32068007554799999</v>
       </c>
       <c r="U5" s="1">
-        <v>0.425600802705</v>
+        <v>0.33377998523000002</v>
       </c>
       <c r="V5" s="1">
-        <v>0.24453599614400001</v>
+        <v>0.16455676681199999</v>
       </c>
       <c r="W5" s="1">
-        <v>0.228946401524</v>
+        <v>0.20615404232500001</v>
       </c>
       <c r="X5" s="1">
-        <v>0.32333439885199999</v>
+        <v>0.27703664256799998</v>
       </c>
       <c r="Y5" s="1">
-        <v>0.34610292920899999</v>
+        <v>0.25353907007600002</v>
       </c>
       <c r="Z5" s="1">
-        <v>0.45625767749099999</v>
+        <v>0.46753328669100003</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
-        <v>-6.76086737828E-2</v>
+        <v>-1.06044262969E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>0.14843505356600001</v>
+        <v>9.5108435595900001E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>4.5954649673699999E-2</v>
+        <v>-6.6542492479500004E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>3.1920558242599997E-2</v>
+        <v>5.63478209439E-2</v>
       </c>
       <c r="F6" s="1">
-        <v>7.49519943593E-2</v>
+        <v>7.8550886780799994E-2</v>
       </c>
       <c r="G6" s="1">
-        <v>-7.26263423297E-2</v>
+        <v>-2.7736658889599999E-2</v>
       </c>
       <c r="H6" s="1">
-        <v>0.17143772037300001</v>
+        <v>0.16523691584200001</v>
       </c>
       <c r="I6" s="1">
-        <v>4.2530759383699997E-2</v>
+        <v>-0.13137241652000001</v>
       </c>
       <c r="J6" s="1">
-        <v>5.0308750919099997E-2</v>
+        <v>3.7563525168200003E-2</v>
       </c>
       <c r="K6" s="1">
-        <v>0.105029377356</v>
+        <v>0.134329880579</v>
       </c>
       <c r="L6" s="1">
-        <v>-7.8916660431900001E-2</v>
+        <v>-2.5836100535399999E-2</v>
       </c>
       <c r="M6" s="1">
-        <v>0.183122339602</v>
+        <v>0.163767718231</v>
       </c>
       <c r="N6" s="1">
-        <v>4.8038438070200001E-2</v>
+        <v>-0.127374577425</v>
       </c>
       <c r="O6" s="1">
-        <v>5.04017363798E-2</v>
+        <v>4.8169724103299998E-2</v>
       </c>
       <c r="P6" s="1">
-        <v>0.107607552573</v>
+        <v>0.13353454148900001</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.23236048588700001</v>
+        <v>0.23140870150500001</v>
       </c>
       <c r="R6" s="1">
-        <v>0.24911849977799999</v>
+        <v>0.15769873651399999</v>
       </c>
       <c r="S6" s="1">
-        <v>0.382882621619</v>
+        <v>0.35416971401800001</v>
       </c>
       <c r="T6" s="1">
-        <v>0.30228495523799997</v>
+        <v>0.32244328503199998</v>
       </c>
       <c r="U6" s="1">
-        <v>0.242510769268</v>
+        <v>5.1420640391500003E-2</v>
       </c>
       <c r="V6" s="1">
-        <v>0.17856697654000001</v>
+        <v>0.19821306831800001</v>
       </c>
       <c r="W6" s="1">
-        <v>0.17536646074000001</v>
+        <v>0.200796137268</v>
       </c>
       <c r="X6" s="1">
-        <v>0.25437057344000003</v>
+        <v>0.167680037852</v>
       </c>
       <c r="Y6" s="1">
-        <v>0.21916875651600001</v>
+        <v>3.9835687132699998E-2</v>
       </c>
       <c r="Z6" s="1">
-        <v>0.49941279846100001</v>
+        <v>0.42706377555199998</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1">
-        <v>-3.6720736554600002E-2</v>
+        <v>-7.4193326688300004E-2</v>
       </c>
       <c r="C7" s="1">
-        <v>8.2222207421099994E-2</v>
+        <v>0.113293110041</v>
       </c>
       <c r="D7" s="1">
-        <v>-9.2337450482600003E-2</v>
+        <v>-4.2755590377600003E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>-3.0108190845400001E-3</v>
+        <v>2.8467863691299999E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>0.102747024838</v>
+        <v>0.10498836508499999</v>
       </c>
       <c r="G7" s="1">
-        <v>-6.713429991E-2</v>
+        <v>-0.101570881502</v>
       </c>
       <c r="H7" s="1">
-        <v>0.15893070638199999</v>
+        <v>0.15932009120999999</v>
       </c>
       <c r="I7" s="1">
-        <v>-6.9230160578200001E-2</v>
+        <v>-0.112442700163</v>
       </c>
       <c r="J7" s="1">
-        <v>5.4677562380400002E-2</v>
+        <v>4.0342681979199997E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>0.17497769714700001</v>
+        <v>0.143737848384</v>
       </c>
       <c r="L7" s="1">
-        <v>-6.7876921584399993E-2</v>
+        <v>-0.105165378441</v>
       </c>
       <c r="M7" s="1">
-        <v>0.15935106423000001</v>
+        <v>0.16404344693699999</v>
       </c>
       <c r="N7" s="1">
-        <v>-8.7124481769899995E-2</v>
+        <v>-0.10459503367</v>
       </c>
       <c r="O7" s="1">
-        <v>4.4960347731899997E-2</v>
+        <v>4.14883552532E-2</v>
       </c>
       <c r="P7" s="1">
-        <v>0.17931915580900001</v>
+        <v>0.148832811812</v>
       </c>
       <c r="Q7" s="1">
-        <v>6.3261004549499997E-2</v>
+        <v>0.231808480634</v>
       </c>
       <c r="R7" s="1">
-        <v>7.0872155155599997E-2</v>
+        <v>0.23560452302599999</v>
       </c>
       <c r="S7" s="1">
-        <v>0.109299190931</v>
+        <v>0.39562730392399997</v>
       </c>
       <c r="T7" s="1">
-        <v>0.124809506436</v>
+        <v>0.34246174276199998</v>
       </c>
       <c r="U7" s="1">
-        <v>0.15977632904899999</v>
+        <v>0.18386749916799999</v>
       </c>
       <c r="V7" s="1">
-        <v>0.103346525188</v>
+        <v>0.20790478054100001</v>
       </c>
       <c r="W7" s="1">
-        <v>0.13012316536900001</v>
+        <v>0.197614419012</v>
       </c>
       <c r="X7" s="1">
-        <v>7.1984238306600001E-2</v>
+        <v>0.21458733369300001</v>
       </c>
       <c r="Y7" s="1">
-        <v>-5.2695577527100003E-2</v>
+        <v>0.12575299671000001</v>
       </c>
       <c r="Z7" s="1">
-        <v>0.210191614118</v>
+        <v>0.49509766183800002</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
-        <v>-1.6488118265000001E-2</v>
+        <v>1.27972393349E-2</v>
       </c>
       <c r="C8" s="1">
-        <v>0.12824485100999999</v>
+        <v>9.9333435595899994E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>1.94722571752E-2</v>
+        <v>-1.5648423933800001E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>9.4210363172200003E-4</v>
+        <v>2.1493241997999998E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>2.1331906877000002E-2</v>
+        <v>5.3213139227699997E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>-3.2147694003500003E-2</v>
+        <v>-4.3124910792200002E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>0.14252024866900001</v>
+        <v>0.12008654291199999</v>
       </c>
       <c r="I8" s="1">
-        <v>-1.37270839432E-2</v>
+        <v>-7.9527338331700004E-2</v>
       </c>
       <c r="J8" s="1">
-        <v>5.92524992257E-2</v>
+        <v>6.9338786579E-2</v>
       </c>
       <c r="K8" s="1">
-        <v>0.10288872969600001</v>
+        <v>0.143377317941</v>
       </c>
       <c r="L8" s="1">
-        <v>-3.0763978085000001E-2</v>
+        <v>-2.9416180581000002E-2</v>
       </c>
       <c r="M8" s="1">
-        <v>0.15512527306599999</v>
+        <v>0.124035076821</v>
       </c>
       <c r="N8" s="1">
-        <v>-4.2635512214599996E-3</v>
+        <v>-6.6539185139999998E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>4.7001999631399997E-2</v>
+        <v>6.0526389963199999E-2</v>
       </c>
       <c r="P8" s="1">
-        <v>8.8182935352999994E-2</v>
+        <v>0.12776758022000001</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.38160384716099999</v>
+        <v>0.33767250296399998</v>
       </c>
       <c r="R8" s="1">
-        <v>0.30157705440600002</v>
+        <v>0.34339401394300001</v>
       </c>
       <c r="S8" s="1">
-        <v>0.57467237850700004</v>
+        <v>0.54630395941599996</v>
       </c>
       <c r="T8" s="1">
-        <v>0.47418522168799998</v>
+        <v>0.47106685096299999</v>
       </c>
       <c r="U8" s="1">
-        <v>0.16967615769700001</v>
+        <v>0.24219110854199999</v>
       </c>
       <c r="V8" s="1">
-        <v>0.41118033285799999</v>
+        <v>0.39241549722199998</v>
       </c>
       <c r="W8" s="1">
-        <v>0.312564122868</v>
+        <v>0.35410415531200001</v>
       </c>
       <c r="X8" s="1">
-        <v>0.37864981797800001</v>
+        <v>0.32469050368300001</v>
       </c>
       <c r="Y8" s="1">
-        <v>0.27623693485599998</v>
+        <v>0.23347305674800001</v>
       </c>
       <c r="Z8" s="1">
-        <v>0.65480164503000005</v>
+        <v>0.68311253797799998</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1">
-        <v>4.4783031349100002E-3</v>
+        <v>7.7053541672200002E-3</v>
       </c>
       <c r="C9" s="1">
-        <v>5.4601585995E-2</v>
+        <v>0.120196039455</v>
       </c>
       <c r="D9" s="1">
-        <v>-7.0926180637200006E-2</v>
+        <v>3.52187458792E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>8.6756108227100004E-2</v>
+        <v>6.6310229242199994E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>9.6336832912900003E-2</v>
+        <v>7.1202294633500002E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>-6.5315451201999997E-2</v>
+        <v>-6.8715119662299998E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>0.14526082011700001</v>
+        <v>0.1524926285</v>
       </c>
       <c r="I9" s="1">
-        <v>-0.20107058605600001</v>
+        <v>-8.0050303628199995E-2</v>
       </c>
       <c r="J9" s="1">
-        <v>7.2294579929E-2</v>
+        <v>8.2899162823500003E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>0.205817779969</v>
+        <v>0.10910674658</v>
       </c>
       <c r="L9" s="1">
-        <v>-5.3984817593900003E-2</v>
+        <v>-5.0557829489599998E-2</v>
       </c>
       <c r="M9" s="1">
-        <v>0.14205782136699999</v>
+        <v>0.156583205364</v>
       </c>
       <c r="N9" s="1">
-        <v>-0.19506845812900001</v>
+        <v>-5.0432100855099998E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>9.0999780303599995E-2</v>
+        <v>8.5473089467700006E-2</v>
       </c>
       <c r="P9" s="1">
-        <v>0.20779353945199999</v>
+        <v>0.10723352139099999</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.247325665995</v>
+        <v>0.342694078618</v>
       </c>
       <c r="R9" s="1">
-        <v>0.20020441309000001</v>
+        <v>0.44199682184200001</v>
       </c>
       <c r="S9" s="1">
-        <v>0.30872375891100001</v>
+        <v>0.54225003558700002</v>
       </c>
       <c r="T9" s="1">
-        <v>0.26368900328900002</v>
+        <v>0.45334718392599999</v>
       </c>
       <c r="U9" s="1">
-        <v>0.16906732767999999</v>
+        <v>0.311521109676</v>
       </c>
       <c r="V9" s="1">
-        <v>0.153381042286</v>
+        <v>0.37484667082299999</v>
       </c>
       <c r="W9" s="1">
-        <v>0.138265934275</v>
+        <v>0.34492040409899999</v>
       </c>
       <c r="X9" s="1">
-        <v>0.119249770385</v>
+        <v>0.42129306594799998</v>
       </c>
       <c r="Y9" s="1">
-        <v>-3.6742809052899998E-2</v>
+        <v>0.32149819761499998</v>
       </c>
       <c r="Z9" s="1">
-        <v>0.38313293113199998</v>
+        <v>0.65791709763100004</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1">
-        <v>-7.4749637834899997E-3</v>
+        <v>-3.3302422801299997E-2</v>
       </c>
       <c r="C10" s="1">
-        <v>7.3570315087599994E-2</v>
+        <v>8.6861373600399999E-2</v>
       </c>
       <c r="D10" s="1">
-        <v>-5.8475676702199997E-2</v>
+        <v>2.9046540744699999E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>4.9425962541599998E-2</v>
+        <v>3.6301700266399999E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>7.9185314700099999E-2</v>
+        <v>8.2655199688699998E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>-2.45873549697E-2</v>
+        <v>-3.5930478955100001E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>7.0131988160800005E-2</v>
+        <v>6.8239982293800003E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>-8.3689787710300001E-2</v>
+        <v>-2.3049542138599999E-2</v>
       </c>
       <c r="J10" s="1">
-        <v>7.2418768250699997E-2</v>
+        <v>8.2964506431400006E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>0.139869360222</v>
+        <v>0.125971475601</v>
       </c>
       <c r="L10" s="1">
-        <v>-2.2061699877000001E-2</v>
+        <v>-3.9506330672499999E-2</v>
       </c>
       <c r="M10" s="1">
-        <v>8.0656417325499996E-2</v>
+        <v>8.2444070325099997E-2</v>
       </c>
       <c r="N10" s="1">
-        <v>-8.6288976945500001E-2</v>
+        <v>-9.3914956343799996E-3</v>
       </c>
       <c r="O10" s="1">
-        <v>7.4227044141899998E-2</v>
+        <v>7.8364702307199996E-2</v>
       </c>
       <c r="P10" s="1">
-        <v>0.13787050108099999</v>
+        <v>0.12767762411799999</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.22861538844400001</v>
+        <v>0.29325302344999998</v>
       </c>
       <c r="R10" s="1">
-        <v>0.13580709846700001</v>
+        <v>0.27513555389900002</v>
       </c>
       <c r="S10" s="1">
-        <v>0.224119019186</v>
+        <v>0.40288890958099999</v>
       </c>
       <c r="T10" s="1">
-        <v>0.221594611</v>
+        <v>0.35103522250899999</v>
       </c>
       <c r="U10" s="1">
-        <v>2.7424427285999999E-2</v>
+        <v>0.23123224673699999</v>
       </c>
       <c r="V10" s="1">
-        <v>0.125851671996</v>
+        <v>0.17957949252700001</v>
       </c>
       <c r="W10" s="1">
-        <v>0.17979040218799999</v>
+        <v>0.177467437935</v>
       </c>
       <c r="X10" s="1">
-        <v>0.110407354428</v>
+        <v>0.26321637234700002</v>
       </c>
       <c r="Y10" s="1">
-        <v>3.7936468679099999E-2</v>
+        <v>0.21133263341299999</v>
       </c>
       <c r="Z10" s="1">
-        <v>0.325753323426</v>
+        <v>0.54110912574299996</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1">
-        <v>-7.0660464790199995E-2</v>
+        <v>-0.209051073601</v>
       </c>
       <c r="C11" s="1">
-        <v>0.12566336856400001</v>
+        <v>0.77097017273400004</v>
       </c>
       <c r="D11" s="1">
-        <v>7.2595324421000001E-2</v>
+        <v>-0.28482687326</v>
       </c>
       <c r="E11" s="1">
-        <v>4.6339745626699999E-2</v>
+        <v>-0.25037132415800001</v>
       </c>
       <c r="F11" s="1">
-        <v>8.2484244205699997E-2</v>
+        <v>0.50660248562999999</v>
       </c>
       <c r="G11" s="1">
-        <v>-8.6749093793699994E-2</v>
+        <v>-9.1662349487699996E-2</v>
       </c>
       <c r="H11" s="1">
-        <v>0.184475696243</v>
+        <v>0.232995933618</v>
       </c>
       <c r="I11" s="1">
-        <v>-5.1531225685099998E-2</v>
+        <v>-6.3257908857600006E-2</v>
       </c>
       <c r="J11" s="1">
-        <v>1.7704089823100001E-2</v>
+        <v>-2.63961174231E-2</v>
       </c>
       <c r="K11" s="1">
-        <v>0.11516116481200001</v>
+        <v>-2.49418048305E-2</v>
       </c>
       <c r="L11" s="1">
-        <v>-9.8021595182299998E-2</v>
+        <v>-0.13822513591999999</v>
       </c>
       <c r="M11" s="1">
-        <v>0.198394222753</v>
+        <v>0.41430255681700001</v>
       </c>
       <c r="N11" s="1">
-        <v>-1.14321233914E-2</v>
+        <v>-0.132159722782</v>
       </c>
       <c r="O11" s="1">
-        <v>3.3050494043900001E-2</v>
+        <v>-8.95873794453E-2</v>
       </c>
       <c r="P11" s="1">
-        <v>0.12544949335</v>
+        <v>0.10979977150299999</v>
       </c>
       <c r="Q11" s="1">
-        <v>0.22444607568300001</v>
+        <v>-4.38867109958E-2</v>
       </c>
       <c r="R11" s="1">
-        <v>0.29189506039000002</v>
+        <v>0.58822227428200002</v>
       </c>
       <c r="S11" s="1">
-        <v>0.38698686446300001</v>
+        <v>-5.4156821288300003E-2</v>
       </c>
       <c r="T11" s="1">
-        <v>0.33792513483300002</v>
+        <v>3.1962119058200002E-3</v>
       </c>
       <c r="U11" s="1">
-        <v>0.33158414439599998</v>
+        <v>2.48294967683E-3</v>
       </c>
       <c r="V11" s="1">
-        <v>0.20622455451300001</v>
+        <v>-0.38289976702200001</v>
       </c>
       <c r="W11" s="1">
-        <v>0.20996610400900001</v>
+        <v>0.59194758621599997</v>
       </c>
       <c r="X11" s="1">
-        <v>0.28404384470799998</v>
+        <v>-0.30571551098100003</v>
       </c>
       <c r="Y11" s="1">
-        <v>0.21347702421299999</v>
+        <v>-0.47826164498399998</v>
       </c>
       <c r="Z11" s="1">
-        <v>0.49443470395299999</v>
+        <v>4.6080798126099998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1">
-        <v>-6.0943001463600002E-2</v>
+        <v>-5.0317598706999998E-2</v>
       </c>
       <c r="C12" s="1">
-        <v>0.17763838615999999</v>
+        <v>6.2933488684199998E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>-2.05294289244E-2</v>
+        <v>-0.14791036896199999</v>
       </c>
       <c r="E12" s="1">
-        <v>5.6290141288299997E-2</v>
+        <v>3.9501523011600002E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>7.9347502315100002E-2</v>
+        <v>0.126412989783</v>
       </c>
       <c r="G12" s="1">
-        <v>-8.7964434996600005E-2</v>
+        <v>-0.10416190784899999</v>
       </c>
       <c r="H12" s="1">
-        <v>0.20990955924999999</v>
+        <v>0.170087553823</v>
       </c>
       <c r="I12" s="1">
-        <v>-9.0183131109100007E-2</v>
+        <v>-0.18164769329899999</v>
       </c>
       <c r="J12" s="1">
-        <v>9.8603631403099995E-2</v>
+        <v>3.7980983155299998E-2</v>
       </c>
       <c r="K12" s="1">
-        <v>0.11211687144099999</v>
+        <v>0.176411075463</v>
       </c>
       <c r="L12" s="1">
-        <v>-8.9531984609900001E-2</v>
+        <v>-0.100479599216</v>
       </c>
       <c r="M12" s="1">
-        <v>0.22287165274099999</v>
+        <v>0.158267583346</v>
       </c>
       <c r="N12" s="1">
-        <v>-7.9696724460700002E-2</v>
+        <v>-0.193620444966</v>
       </c>
       <c r="O12" s="1">
-        <v>9.6855214829400002E-2</v>
+        <v>4.3051228816999999E-2</v>
       </c>
       <c r="P12" s="1">
-        <v>0.114587301192</v>
+        <v>0.18277846148400001</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.30486368692799998</v>
+        <v>0.13858605153600001</v>
       </c>
       <c r="R12" s="1">
-        <v>0.34977602885699999</v>
+        <v>0.156678341226</v>
       </c>
       <c r="S12" s="1">
-        <v>0.44582551193499997</v>
+        <v>0.168963023144</v>
       </c>
       <c r="T12" s="1">
-        <v>0.37714996334200002</v>
+        <v>0.130971095368</v>
       </c>
       <c r="U12" s="1">
-        <v>0.27836945324500001</v>
+        <v>0.11836752268</v>
       </c>
       <c r="V12" s="1">
-        <v>0.26461320972800001</v>
+        <v>0.105679128469</v>
       </c>
       <c r="W12" s="1">
-        <v>0.27902810883500001</v>
+        <v>0.111552146031</v>
       </c>
       <c r="X12" s="1">
-        <v>0.328096302723</v>
+        <v>0.12158260683</v>
       </c>
       <c r="Y12" s="1">
-        <v>0.28577752312499999</v>
+        <v>-2.58537155045E-2</v>
       </c>
       <c r="Z12" s="1">
-        <v>0.55781539900999999</v>
+        <v>0.35006815432900001</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1">
-        <v>-3.2801876895500001E-2</v>
+        <v>-5.65811451592E-2</v>
       </c>
       <c r="C13" s="1">
-        <v>6.2564003163799994E-2</v>
+        <v>8.2523404454699995E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>9.78841048055E-3</v>
+        <v>-0.107180939446</v>
       </c>
       <c r="E13" s="1">
-        <v>6.7907279451699998E-2</v>
+        <v>1.5853974583500002E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>7.4973650728200003E-2</v>
+        <v>0.129297297093</v>
       </c>
       <c r="G13" s="1">
-        <v>-7.9994533267600004E-2</v>
+        <v>-8.2474190042500006E-2</v>
       </c>
       <c r="H13" s="1">
-        <v>0.145783034901</v>
+        <v>0.13982330652399999</v>
       </c>
       <c r="I13" s="1">
-        <v>4.1810599625E-2</v>
+        <v>-0.17548806334</v>
       </c>
       <c r="J13" s="1">
-        <v>2.9822947080400002E-2</v>
+        <v>2.78728074035E-2</v>
       </c>
       <c r="K13" s="1">
-        <v>9.7750612035000004E-2</v>
+        <v>0.184084712663</v>
       </c>
       <c r="L13" s="1">
-        <v>-7.7336395777899997E-2</v>
+        <v>-8.5534685890800002E-2</v>
       </c>
       <c r="M13" s="1">
-        <v>0.141882067409</v>
+        <v>0.141123880688</v>
       </c>
       <c r="N13" s="1">
-        <v>3.7891371477800001E-2</v>
+        <v>-0.178184516264</v>
       </c>
       <c r="O13" s="1">
-        <v>4.7833759067999998E-2</v>
+        <v>2.8005992409100001E-2</v>
       </c>
       <c r="P13" s="1">
-        <v>0.10641215232200001</v>
+        <v>0.19181706549899999</v>
       </c>
       <c r="Q13" s="1">
-        <v>0.27920346198599999</v>
+        <v>0.19124211172899999</v>
       </c>
       <c r="R13" s="1">
-        <v>0.31881210916399999</v>
+        <v>0.15516921735799999</v>
       </c>
       <c r="S13" s="1">
-        <v>0.32153007002400003</v>
+        <v>0.22082391967199999</v>
       </c>
       <c r="T13" s="1">
-        <v>0.29541794354599998</v>
+        <v>0.18553876906299999</v>
       </c>
       <c r="U13" s="1">
-        <v>0.30436468460299998</v>
+        <v>9.8063302964099999E-2</v>
       </c>
       <c r="V13" s="1">
-        <v>0.16602843689399999</v>
+        <v>0.104259113027</v>
       </c>
       <c r="W13" s="1">
-        <v>0.140634922202</v>
+        <v>0.103927754085</v>
       </c>
       <c r="X13" s="1">
-        <v>0.26291910826300002</v>
+        <v>0.115917879712</v>
       </c>
       <c r="Y13" s="1">
-        <v>0.22612603824700001</v>
+        <v>-4.5541788022599996E-3</v>
       </c>
       <c r="Z13" s="1">
-        <v>0.45380355293000002</v>
+        <v>0.36803728026100002</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1">
-        <v>-7.4633277030100004E-2</v>
+        <v>-3.6176171114899999E-2</v>
       </c>
       <c r="C14" s="1">
-        <v>0.19075293416899999</v>
+        <v>0.10728780651600001</v>
       </c>
       <c r="D14" s="1">
-        <v>4.5293908728600001E-2</v>
+        <v>-8.3949064858499997E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>8.2179955708499994E-2</v>
+        <v>5.5413402297000001E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>0.106061164528</v>
+        <v>8.4466064713699995E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>-0.103373911225</v>
+        <v>-5.2021159062799999E-2</v>
       </c>
       <c r="H14" s="1">
-        <v>0.22862546036100001</v>
+        <v>0.146241697453</v>
       </c>
       <c r="I14" s="1">
-        <v>-1.28923038541E-2</v>
+        <v>-9.8212232107199995E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>0.13563843952999999</v>
+        <v>2.51132952531E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>0.170629249407</v>
+        <v>0.11965675519299999</v>
       </c>
       <c r="L14" s="1">
-        <v>-0.10708642817400001</v>
+        <v>-5.4733292934599997E-2</v>
       </c>
       <c r="M14" s="1">
-        <v>0.245022854811</v>
+        <v>0.15564463216400001</v>
       </c>
       <c r="N14" s="1">
-        <v>3.9759334268099997E-3</v>
+        <v>-0.108540128007</v>
       </c>
       <c r="O14" s="1">
-        <v>0.13555231832100001</v>
+        <v>3.9081165472699998E-2</v>
       </c>
       <c r="P14" s="1">
-        <v>0.17138108756699999</v>
+        <v>0.126251244766</v>
       </c>
       <c r="Q14" s="1">
-        <v>0.211925832157</v>
+        <v>0.18892738009500001</v>
       </c>
       <c r="R14" s="1">
-        <v>0.235376190234</v>
+        <v>0.165295041951</v>
       </c>
       <c r="S14" s="1">
-        <v>0.36583828063000001</v>
+        <v>0.165122885054</v>
       </c>
       <c r="T14" s="1">
-        <v>0.29309070420700001</v>
+        <v>0.14155111829899999</v>
       </c>
       <c r="U14" s="1">
-        <v>0.25458062889299998</v>
+        <v>8.7800260714500006E-2</v>
       </c>
       <c r="V14" s="1">
-        <v>0.20777078356199999</v>
+        <v>6.5329074720800004E-2</v>
       </c>
       <c r="W14" s="1">
-        <v>0.182330782469</v>
+        <v>6.6682475135199995E-2</v>
       </c>
       <c r="X14" s="1">
-        <v>0.222273511191</v>
+        <v>8.6708632174599995E-2</v>
       </c>
       <c r="Y14" s="1">
-        <v>0.16699306143199999</v>
+        <v>5.1881835328299996E-3</v>
       </c>
       <c r="Z14" s="1">
-        <v>0.49504912022699998</v>
+        <v>0.32156897142399998</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
-        <v>-1.06044262969E-2</v>
+        <v>-3.6720736554600002E-2</v>
       </c>
       <c r="C15" s="1">
-        <v>9.5108435595900001E-2</v>
+        <v>8.2222207421099994E-2</v>
       </c>
       <c r="D15" s="1">
-        <v>-6.6542492479500004E-2</v>
+        <v>-9.2337450482600003E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>5.63478209439E-2</v>
+        <v>-3.0108190845400001E-3</v>
       </c>
       <c r="F15" s="1">
-        <v>7.8550886780799994E-2</v>
+        <v>0.102747024838</v>
       </c>
       <c r="G15" s="1">
-        <v>-2.7736658889599999E-2</v>
+        <v>-6.713429991E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>0.16523691584200001</v>
+        <v>0.15893070638199999</v>
       </c>
       <c r="I15" s="1">
-        <v>-0.13137241652000001</v>
+        <v>-6.9230160578200001E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>3.7563525168200003E-2</v>
+        <v>5.4677562380400002E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>0.134329880579</v>
+        <v>0.17497769714700001</v>
       </c>
       <c r="L15" s="1">
-        <v>-2.5836100535399999E-2</v>
+        <v>-6.7876921584399993E-2</v>
       </c>
       <c r="M15" s="1">
-        <v>0.163767718231</v>
+        <v>0.15935106423000001</v>
       </c>
       <c r="N15" s="1">
-        <v>-0.127374577425</v>
+        <v>-8.7124481769899995E-2</v>
       </c>
       <c r="O15" s="1">
-        <v>4.8169724103299998E-2</v>
+        <v>4.4960347731899997E-2</v>
       </c>
       <c r="P15" s="1">
-        <v>0.13353454148900001</v>
+        <v>0.17931915580900001</v>
       </c>
       <c r="Q15" s="1">
-        <v>0.23140870150500001</v>
+        <v>6.3261004549499997E-2</v>
       </c>
       <c r="R15" s="1">
-        <v>0.15769873651399999</v>
+        <v>7.0872155155599997E-2</v>
       </c>
       <c r="S15" s="1">
-        <v>0.35416971401800001</v>
+        <v>0.109299190931</v>
       </c>
       <c r="T15" s="1">
-        <v>0.32244328503199998</v>
+        <v>0.124809506436</v>
       </c>
       <c r="U15" s="1">
-        <v>5.1420640391500003E-2</v>
+        <v>0.15977632904899999</v>
       </c>
       <c r="V15" s="1">
-        <v>0.19821306831800001</v>
+        <v>0.103346525188</v>
       </c>
       <c r="W15" s="1">
-        <v>0.200796137268</v>
+        <v>0.13012316536900001</v>
       </c>
       <c r="X15" s="1">
-        <v>0.167680037852</v>
+        <v>7.1984238306600001E-2</v>
       </c>
       <c r="Y15" s="1">
-        <v>3.9835687132699998E-2</v>
+        <v>-5.2695577527100003E-2</v>
       </c>
       <c r="Z15" s="1">
-        <v>0.42706377555199998</v>
+        <v>0.210191614118</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1">
-        <v>-3.5879471521699999E-2</v>
+        <v>1.1854391374E-2</v>
       </c>
       <c r="C16" s="1">
-        <v>7.8194460742399996E-2</v>
+        <v>9.0747447100999995E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>-2.69453151256E-2</v>
+        <v>-0.109544221678</v>
       </c>
       <c r="E16" s="1">
-        <v>1.0251080094700001E-2</v>
+        <v>2.9482936731100001E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>8.6281791867300006E-2</v>
+        <v>0.12696369347700001</v>
       </c>
       <c r="G16" s="1">
-        <v>-0.101495901863</v>
+        <v>-7.3873110560799995E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>0.134426675548</v>
+        <v>0.16595289915899999</v>
       </c>
       <c r="I16" s="1">
-        <v>-3.1216033106400001E-2</v>
+        <v>-0.22900811751700001</v>
       </c>
       <c r="J16" s="1">
-        <v>4.4604320748700002E-3</v>
+        <v>1.47016021681E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>9.8009437699000002E-2</v>
+        <v>0.180356358021</v>
       </c>
       <c r="L16" s="1">
-        <v>-9.5125428482300003E-2</v>
+        <v>-6.1000664657300002E-2</v>
       </c>
       <c r="M16" s="1">
-        <v>0.135893863955</v>
+        <v>0.17052935108600001</v>
       </c>
       <c r="N16" s="1">
-        <v>-3.4319069747100001E-2</v>
+        <v>-0.230701438599</v>
       </c>
       <c r="O16" s="1">
-        <v>6.9089915596399999E-3</v>
+        <v>2.11755260057E-2</v>
       </c>
       <c r="P16" s="1">
-        <v>0.108356089467</v>
+        <v>0.19332128844999999</v>
       </c>
       <c r="Q16" s="1">
-        <v>0.14645153434899999</v>
+        <v>0.229076797272</v>
       </c>
       <c r="R16" s="1">
-        <v>0.118555121115</v>
+        <v>0.22870224263300001</v>
       </c>
       <c r="S16" s="1">
-        <v>0.220097621258</v>
+        <v>0.21645320425799999</v>
       </c>
       <c r="T16" s="1">
-        <v>0.178157457524</v>
+        <v>0.19705574049499999</v>
       </c>
       <c r="U16" s="1">
-        <v>0.119987181783</v>
+        <v>0.178180672027</v>
       </c>
       <c r="V16" s="1">
-        <v>0.109996137902</v>
+        <v>0.12611712524800001</v>
       </c>
       <c r="W16" s="1">
-        <v>0.11174905912499999</v>
+        <v>0.14619254273000001</v>
       </c>
       <c r="X16" s="1">
-        <v>8.9898101342700001E-2</v>
+        <v>0.17472378746299999</v>
       </c>
       <c r="Y16" s="1">
-        <v>1.6741901468899999E-2</v>
+        <v>-6.7599082670600002E-3</v>
       </c>
       <c r="Z16" s="1">
-        <v>0.37171952956400001</v>
+        <v>0.355910920676</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1">
-        <v>-6.9100301815299997E-2</v>
+        <v>-4.6362763452400001E-2</v>
       </c>
       <c r="C17" s="1">
-        <v>0.10345943905</v>
+        <v>9.1678388138100003E-2</v>
       </c>
       <c r="D17" s="1">
-        <v>-1.0571937721099999E-2</v>
+        <v>-0.14665480549500001</v>
       </c>
       <c r="E17" s="1">
-        <v>6.9122577524000001E-2</v>
+        <v>5.2660642245500003E-2</v>
       </c>
       <c r="F17" s="1">
-        <v>0.100349349404</v>
+        <v>0.121185620085</v>
       </c>
       <c r="G17" s="1">
-        <v>-0.105268807016</v>
+        <v>-0.13983768101499999</v>
       </c>
       <c r="H17" s="1">
-        <v>0.18209078874699999</v>
+        <v>0.24253301530800001</v>
       </c>
       <c r="I17" s="1">
-        <v>-0.104644736303</v>
+        <v>-0.255244460058</v>
       </c>
       <c r="J17" s="1">
-        <v>4.9527271412299997E-2</v>
+        <v>1.2710034749500001E-3</v>
       </c>
       <c r="K17" s="1">
-        <v>0.17445594262700001</v>
+        <v>0.20935788267200001</v>
       </c>
       <c r="L17" s="1">
-        <v>-0.109255149339</v>
+        <v>-0.13196519151</v>
       </c>
       <c r="M17" s="1">
-        <v>0.18358123360699999</v>
+        <v>0.232490737945</v>
       </c>
       <c r="N17" s="1">
-        <v>-8.9094310606300006E-2</v>
+        <v>-0.26056082015900001</v>
       </c>
       <c r="O17" s="1">
-        <v>6.3725723678699997E-2</v>
+        <v>1.77899341702E-2</v>
       </c>
       <c r="P17" s="1">
-        <v>0.17626849044699999</v>
+        <v>0.21400803189000001</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.217924747344</v>
+        <v>0.18665646704</v>
       </c>
       <c r="R17" s="1">
-        <v>0.22376549667599999</v>
+        <v>0.26202315465199999</v>
       </c>
       <c r="S17" s="1">
-        <v>0.357145373993</v>
+        <v>0.214212157938</v>
       </c>
       <c r="T17" s="1">
-        <v>0.31932297472900001</v>
+        <v>0.16601334752800001</v>
       </c>
       <c r="U17" s="1">
-        <v>0.29636668298199997</v>
+        <v>0.12084235552</v>
       </c>
       <c r="V17" s="1">
-        <v>0.19405140334500001</v>
+        <v>9.8716921218700002E-2</v>
       </c>
       <c r="W17" s="1">
-        <v>0.19759564192599999</v>
+        <v>0.169134016538</v>
       </c>
       <c r="X17" s="1">
-        <v>0.20434790579000001</v>
+        <v>0.11900167495400001</v>
       </c>
       <c r="Y17" s="1">
-        <v>9.5538906489600006E-2</v>
+        <v>2.2421252900100001E-2</v>
       </c>
       <c r="Z17" s="1">
-        <v>0.45569815251000001</v>
+        <v>0.36078528477100003</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1">
-        <v>-3.8345240647599997E-2</v>
+        <v>-5.5869371492199997E-2</v>
       </c>
       <c r="C18" s="1">
-        <v>6.9444446596800005E-2</v>
+        <v>0.13171469455199999</v>
       </c>
       <c r="D18" s="1">
-        <v>-6.9741999434299998E-2</v>
+        <v>-9.1916054290499996E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>5.2320401696499999E-2</v>
+        <v>2.6702737865599999E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>0.105186273025</v>
+        <v>6.0182381336799998E-2</v>
       </c>
       <c r="G18" s="1">
-        <v>-7.1488258945300004E-2</v>
+        <v>-5.7161330941600003E-2</v>
       </c>
       <c r="H18" s="1">
-        <v>0.153980502953</v>
+        <v>0.22902526120700001</v>
       </c>
       <c r="I18" s="1">
-        <v>-0.20416884763900001</v>
+        <v>-0.106273439555</v>
       </c>
       <c r="J18" s="1">
-        <v>3.0877228387100001E-2</v>
+        <v>2.5088852395699999E-2</v>
       </c>
       <c r="K18" s="1">
-        <v>0.18263973725999999</v>
+        <v>7.1164212683700004E-2</v>
       </c>
       <c r="L18" s="1">
-        <v>-7.1856493866599994E-2</v>
+        <v>-6.4503295074400002E-2</v>
       </c>
       <c r="M18" s="1">
-        <v>0.15049238186200001</v>
+        <v>0.22984879934800001</v>
       </c>
       <c r="N18" s="1">
-        <v>-0.19234149195899999</v>
+        <v>-0.11620690513199999</v>
       </c>
       <c r="O18" s="1">
-        <v>4.2648868553399999E-2</v>
+        <v>2.8986654413299999E-2</v>
       </c>
       <c r="P18" s="1">
-        <v>0.18593148695699999</v>
+        <v>7.7411889417000002E-2</v>
       </c>
       <c r="Q18" s="1">
-        <v>0.24794692906599999</v>
+        <v>0.21345489364799999</v>
       </c>
       <c r="R18" s="1">
-        <v>0.233259913111</v>
+        <v>0.26201130450100002</v>
       </c>
       <c r="S18" s="1">
-        <v>0.26510829057500002</v>
+        <v>0.26494998506099998</v>
       </c>
       <c r="T18" s="1">
-        <v>0.248704084873</v>
+        <v>0.23457903312799999</v>
       </c>
       <c r="U18" s="1">
-        <v>0.19475649623999999</v>
+        <v>0.150036602549</v>
       </c>
       <c r="V18" s="1">
-        <v>0.15183802320500001</v>
+        <v>0.14590969089899999</v>
       </c>
       <c r="W18" s="1">
-        <v>0.143249106509</v>
+        <v>0.138640244538</v>
       </c>
       <c r="X18" s="1">
-        <v>0.17348168556499999</v>
+        <v>0.181119234785</v>
       </c>
       <c r="Y18" s="1">
-        <v>5.65548299709E-2</v>
+        <v>9.9304238517199994E-2</v>
       </c>
       <c r="Z18" s="1">
-        <v>0.39486474678299999</v>
+        <v>0.419374042477</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1">
-        <v>-4.7630537009899998E-2</v>
+        <v>-2.13531752727E-2</v>
       </c>
       <c r="C19" s="1">
-        <v>0.12403377466399999</v>
+        <v>0.101551492715</v>
       </c>
       <c r="D19" s="1">
-        <v>6.6582926381299999E-3</v>
+        <v>-9.52045242066E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>6.6993104952300001E-2</v>
+        <v>4.5497156405699998E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>6.8742972567800001E-2</v>
+        <v>7.4726358121200001E-2</v>
       </c>
       <c r="G19" s="1">
-        <v>-9.6750189361399994E-2</v>
+        <v>-7.3107431933899999E-2</v>
       </c>
       <c r="H19" s="1">
-        <v>0.205758351162</v>
+        <v>0.15898512776400001</v>
       </c>
       <c r="I19" s="1">
-        <v>-4.7537484465099998E-2</v>
+        <v>-0.22014427673199999</v>
       </c>
       <c r="J19" s="1">
-        <v>7.9918579742099996E-2</v>
+        <v>2.2170921381500001E-2</v>
       </c>
       <c r="K19" s="1">
-        <v>0.16189080978100001</v>
+        <v>0.18040040163599999</v>
       </c>
       <c r="L19" s="1">
-        <v>-9.4559249476599994E-2</v>
+        <v>-6.8130322106099997E-2</v>
       </c>
       <c r="M19" s="1">
-        <v>0.20856677357299999</v>
+        <v>0.16726742536299999</v>
       </c>
       <c r="N19" s="1">
-        <v>-3.6578151633400002E-2</v>
+        <v>-0.21586471172999999</v>
       </c>
       <c r="O19" s="1">
-        <v>8.7235464533599996E-2</v>
+        <v>3.4117413798999997E-2</v>
       </c>
       <c r="P19" s="1">
-        <v>0.15460531138899999</v>
+        <v>0.17577134414199999</v>
       </c>
       <c r="Q19" s="1">
-        <v>0.23399070411199999</v>
+        <v>0.19849261846899999</v>
       </c>
       <c r="R19" s="1">
-        <v>0.25661056759299999</v>
+        <v>0.21668326603499999</v>
       </c>
       <c r="S19" s="1">
-        <v>0.38386499456599998</v>
+        <v>0.19207543757000001</v>
       </c>
       <c r="T19" s="1">
-        <v>0.34599419833099998</v>
+        <v>0.168375355039</v>
       </c>
       <c r="U19" s="1">
-        <v>0.320162659214</v>
+        <v>0.125638752982</v>
       </c>
       <c r="V19" s="1">
-        <v>0.204834523602</v>
+        <v>0.14149919411699999</v>
       </c>
       <c r="W19" s="1">
-        <v>0.19649582228199999</v>
+        <v>0.12434125518</v>
       </c>
       <c r="X19" s="1">
-        <v>0.22139658206099999</v>
+        <v>0.106772231774</v>
       </c>
       <c r="Y19" s="1">
-        <v>0.11429282187000001</v>
+        <v>-4.3429612474300001E-2</v>
       </c>
       <c r="Z19" s="1">
-        <v>0.50061972563799995</v>
+        <v>0.32710994249600001</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1">
-        <v>1.1854391374E-2</v>
+        <v>-3.5879471521699999E-2</v>
       </c>
       <c r="C20" s="1">
-        <v>9.0747447100999995E-2</v>
+        <v>7.8194460742399996E-2</v>
       </c>
       <c r="D20" s="1">
-        <v>-0.109544221678</v>
+        <v>-2.69453151256E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>2.9482936731100001E-2</v>
+        <v>1.0251080094700001E-2</v>
       </c>
       <c r="F20" s="1">
-        <v>0.12696369347700001</v>
+        <v>8.6281791867300006E-2</v>
       </c>
       <c r="G20" s="1">
-        <v>-7.3873110560799995E-2</v>
+        <v>-0.101495901863</v>
       </c>
       <c r="H20" s="1">
-        <v>0.16595289915899999</v>
+        <v>0.134426675548</v>
       </c>
       <c r="I20" s="1">
-        <v>-0.22900811751700001</v>
+        <v>-3.1216033106400001E-2</v>
       </c>
       <c r="J20" s="1">
-        <v>1.47016021681E-2</v>
+        <v>4.4604320748700002E-3</v>
       </c>
       <c r="K20" s="1">
-        <v>0.180356358021</v>
+        <v>9.8009437699000002E-2</v>
       </c>
       <c r="L20" s="1">
-        <v>-6.1000664657300002E-2</v>
+        <v>-9.5125428482300003E-2</v>
       </c>
       <c r="M20" s="1">
-        <v>0.17052935108600001</v>
+        <v>0.135893863955</v>
       </c>
       <c r="N20" s="1">
-        <v>-0.230701438599</v>
+        <v>-3.4319069747100001E-2</v>
       </c>
       <c r="O20" s="1">
-        <v>2.11755260057E-2</v>
+        <v>6.9089915596399999E-3</v>
       </c>
       <c r="P20" s="1">
-        <v>0.19332128844999999</v>
+        <v>0.108356089467</v>
       </c>
       <c r="Q20" s="1">
-        <v>0.229076797272</v>
+        <v>0.14645153434899999</v>
       </c>
       <c r="R20" s="1">
-        <v>0.22870224263300001</v>
+        <v>0.118555121115</v>
       </c>
       <c r="S20" s="1">
-        <v>0.21645320425799999</v>
+        <v>0.220097621258</v>
       </c>
       <c r="T20" s="1">
-        <v>0.19705574049499999</v>
+        <v>0.178157457524</v>
       </c>
       <c r="U20" s="1">
-        <v>0.178180672027</v>
+        <v>0.119987181783</v>
       </c>
       <c r="V20" s="1">
-        <v>0.12611712524800001</v>
+        <v>0.109996137902</v>
       </c>
       <c r="W20" s="1">
-        <v>0.14619254273000001</v>
+        <v>0.11174905912499999</v>
       </c>
       <c r="X20" s="1">
-        <v>0.17472378746299999</v>
+        <v>8.9898101342700001E-2</v>
       </c>
       <c r="Y20" s="1">
-        <v>-6.7599082670600002E-3</v>
+        <v>1.6741901468899999E-2</v>
       </c>
       <c r="Z20" s="1">
-        <v>0.355910920676</v>
+        <v>0.37171952956400001</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1">
-        <v>1.48431358416E-2</v>
+        <v>-3.3872842694200003E-2</v>
       </c>
       <c r="C21" s="1">
-        <v>9.05679933134E-2</v>
+        <v>0.104811256162</v>
       </c>
       <c r="D21" s="1">
-        <v>-2.4282608886699999E-2</v>
+        <v>-8.40042587511E-2</v>
       </c>
       <c r="E21" s="1">
-        <v>4.52103570154E-2</v>
+        <v>3.8097180386100001E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>5.6628249168600001E-2</v>
+        <v>7.3828947253100005E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>-1.8472459240499998E-2</v>
+        <v>-9.8635019504299995E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>0.19359720184500001</v>
+        <v>0.19255424566900001</v>
       </c>
       <c r="I21" s="1">
-        <v>-8.5184505789100001E-2</v>
+        <v>-0.207937538353</v>
       </c>
       <c r="J21" s="1">
-        <v>0.13426274342200001</v>
+        <v>2.39205209842E-2</v>
       </c>
       <c r="K21" s="1">
-        <v>0.13689826648600001</v>
+        <v>0.15360217407000001</v>
       </c>
       <c r="L21" s="1">
-        <v>-9.8983861253499998E-3</v>
+        <v>-9.3229561929400004E-2</v>
       </c>
       <c r="M21" s="1">
-        <v>0.180412019397</v>
+        <v>0.19447959614099999</v>
       </c>
       <c r="N21" s="1">
-        <v>-7.4543514194199995E-2</v>
+        <v>-0.200603692088</v>
       </c>
       <c r="O21" s="1">
-        <v>0.119739416936</v>
+        <v>3.2257824113000003E-2</v>
       </c>
       <c r="P21" s="1">
-        <v>0.12529827050600001</v>
+        <v>0.15199987561700001</v>
       </c>
       <c r="Q21" s="1">
-        <v>0.408899182842</v>
+        <v>0.22082916900499999</v>
       </c>
       <c r="R21" s="1">
-        <v>0.37218165518099999</v>
+        <v>0.25978083088199999</v>
       </c>
       <c r="S21" s="1">
-        <v>0.61590521145699995</v>
+        <v>0.25589919743700001</v>
       </c>
       <c r="T21" s="1">
-        <v>0.52396003786500001</v>
+        <v>0.22894832336400001</v>
       </c>
       <c r="U21" s="1">
-        <v>0.265712036373</v>
+        <v>0.12292803222699999</v>
       </c>
       <c r="V21" s="1">
-        <v>0.44608898122399998</v>
+        <v>0.15551247132000001</v>
       </c>
       <c r="W21" s="1">
-        <v>0.375226589326</v>
+        <v>0.151278967254</v>
       </c>
       <c r="X21" s="1">
-        <v>0.36440152265600001</v>
+        <v>0.137623573818</v>
       </c>
       <c r="Y21" s="1">
-        <v>0.27139960262700003</v>
+        <v>5.2483237512700003E-2</v>
       </c>
       <c r="Z21" s="1">
-        <v>0.70784472000300003</v>
+        <v>0.38974621171200002</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1">
-        <v>3.2281060828299998E-2</v>
+        <v>-3.7813053008699998E-2</v>
       </c>
       <c r="C22" s="1">
-        <v>0.118066094092</v>
+        <v>9.7681366783599996E-2</v>
       </c>
       <c r="D22" s="1">
-        <v>-2.61392593787E-2</v>
+        <v>-7.9157589987099999E-2</v>
       </c>
       <c r="E22" s="1">
-        <v>-1.9111785090699999E-2</v>
+        <v>7.7245938801999994E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>5.7240431898099998E-2</v>
+        <v>9.3039134756700004E-2</v>
       </c>
       <c r="G22" s="1">
-        <v>-4.3332770453599997E-2</v>
+        <v>-9.6200206600900007E-2</v>
       </c>
       <c r="H22" s="1">
-        <v>0.110953346105</v>
+        <v>0.19726526125800001</v>
       </c>
       <c r="I22" s="1">
-        <v>-3.5959192133200001E-2</v>
+        <v>-0.17023596491199999</v>
       </c>
       <c r="J22" s="1">
-        <v>2.5688419357299999E-2</v>
+        <v>3.2165474704699999E-2</v>
       </c>
       <c r="K22" s="1">
-        <v>8.9080983824200002E-2</v>
+        <v>0.15504665208499999</v>
       </c>
       <c r="L22" s="1">
-        <v>-2.3372574398200001E-2</v>
+        <v>-9.36146199245E-2</v>
       </c>
       <c r="M22" s="1">
-        <v>0.12483179556100001</v>
+        <v>0.19877431251399999</v>
       </c>
       <c r="N22" s="1">
-        <v>-3.6545028697799999E-2</v>
+        <v>-0.16981258885</v>
       </c>
       <c r="O22" s="1">
-        <v>1.39513960622E-2</v>
+        <v>5.3065523246200001E-2</v>
       </c>
       <c r="P22" s="1">
-        <v>8.8098243068400001E-2</v>
+        <v>0.161727526958</v>
       </c>
       <c r="Q22" s="1">
-        <v>0.31262000576799998</v>
+        <v>0.175028240197</v>
       </c>
       <c r="R22" s="1">
-        <v>0.28923731277100001</v>
+        <v>0.137746853192</v>
       </c>
       <c r="S22" s="1">
-        <v>0.46189842037000001</v>
+        <v>0.213329747771</v>
       </c>
       <c r="T22" s="1">
-        <v>0.41103762754200002</v>
+        <v>0.18739182988399999</v>
       </c>
       <c r="U22" s="1">
-        <v>0.25553471360199997</v>
+        <v>7.9642384087699997E-2</v>
       </c>
       <c r="V22" s="1">
-        <v>0.26737842477899998</v>
+        <v>0.138809134004</v>
       </c>
       <c r="W22" s="1">
-        <v>0.24036802603499999</v>
+        <v>0.146353947983</v>
       </c>
       <c r="X22" s="1">
-        <v>0.27359070037400002</v>
+        <v>0.105778131044</v>
       </c>
       <c r="Y22" s="1">
-        <v>0.197283823286</v>
+        <v>-3.5151933079199997E-2</v>
       </c>
       <c r="Z22" s="1">
-        <v>0.57894027108699997</v>
+        <v>0.30549079383700001</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1">
-        <v>4.0708538595600002E-2</v>
+        <v>-4.3922932951300002E-2</v>
       </c>
       <c r="C23" s="1">
-        <v>0.137263541554</v>
+        <v>0.189989091272</v>
       </c>
       <c r="D23" s="1">
-        <v>-1.25530861541E-2</v>
+        <v>3.9868948970999997E-2</v>
       </c>
       <c r="E23" s="1">
-        <v>1.0187559591199999E-2</v>
+        <v>0.105061792652</v>
       </c>
       <c r="F23" s="1">
-        <v>5.43337271819E-2</v>
+        <v>0.155637219662</v>
       </c>
       <c r="G23" s="1">
-        <v>6.0322280173200002E-2</v>
+        <v>-9.4451829262199999E-2</v>
       </c>
       <c r="H23" s="1">
-        <v>0.28770548238999999</v>
+        <v>0.26281409817899998</v>
       </c>
       <c r="I23" s="1">
-        <v>2.5015296044899999E-3</v>
+        <v>3.4238525576100001E-3</v>
       </c>
       <c r="J23" s="1">
-        <v>-6.8272695861100003E-3</v>
+        <v>0.19813795920499999</v>
       </c>
       <c r="K23" s="1">
-        <v>9.3098671232200003E-2</v>
+        <v>0.26133318276099998</v>
       </c>
       <c r="L23" s="1">
-        <v>6.34243017144E-2</v>
+        <v>-8.8377439138800001E-2</v>
       </c>
       <c r="M23" s="1">
-        <v>0.28082063420199999</v>
+        <v>0.26606878416800001</v>
       </c>
       <c r="N23" s="1">
-        <v>-2.9231954077999999E-3</v>
+        <v>1.45897276569E-2</v>
       </c>
       <c r="O23" s="1">
-        <v>-1.50081416636E-3</v>
+        <v>0.189282174208</v>
       </c>
       <c r="P23" s="1">
-        <v>9.4668588817800006E-2</v>
+        <v>0.254717344929</v>
       </c>
       <c r="Q23" s="1">
-        <v>0.33050073022900001</v>
+        <v>0.29605161783099998</v>
       </c>
       <c r="R23" s="1">
-        <v>0.19055990326200001</v>
+        <v>0.33337413213099998</v>
       </c>
       <c r="S23" s="1">
-        <v>0.34441990162699998</v>
+        <v>0.47805313856100001</v>
       </c>
       <c r="T23" s="1">
-        <v>0.37268274161999998</v>
+        <v>0.38998444216799999</v>
       </c>
       <c r="U23" s="1">
-        <v>0.19271740228500001</v>
+        <v>0.40176231948800001</v>
       </c>
       <c r="V23" s="1">
-        <v>0.26758386458700001</v>
+        <v>0.37004785445600002</v>
       </c>
       <c r="W23" s="1">
-        <v>0.210390565334</v>
+        <v>0.33391683234300001</v>
       </c>
       <c r="X23" s="1">
-        <v>8.0771238575100004E-2</v>
+        <v>0.31379360285399999</v>
       </c>
       <c r="Y23" s="1">
-        <v>3.9671533752399998E-2</v>
+        <v>0.22758890430299999</v>
       </c>
       <c r="Z23" s="1">
-        <v>0.493719640972</v>
+        <v>0.72572284111300001</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1">
-        <v>-6.7358902629599995E-2</v>
+        <v>-6.3589077384599998E-2</v>
       </c>
       <c r="C24" s="1">
-        <v>0.158632512856</v>
+        <v>0.14433746606600001</v>
       </c>
       <c r="D24" s="1">
-        <v>3.3797436588600002E-2</v>
+        <v>6.8918933092099996E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>6.0146720432199999E-2</v>
+        <v>5.4798408131699998E-2</v>
       </c>
       <c r="F24" s="1">
-        <v>8.9313858498100002E-2</v>
+        <v>7.4253012043399999E-2</v>
       </c>
       <c r="G24" s="1">
-        <v>-9.6386326904099998E-2</v>
+        <v>-0.14340111166399999</v>
       </c>
       <c r="H24" s="1">
-        <v>0.23630622872599999</v>
+        <v>0.19022263852099999</v>
       </c>
       <c r="I24" s="1">
-        <v>-4.0791023134399999E-4</v>
+        <v>-0.13699852162000001</v>
       </c>
       <c r="J24" s="1">
-        <v>0.105186071827</v>
+        <v>0.19128508995499999</v>
       </c>
       <c r="K24" s="1">
-        <v>0.128614743192</v>
+        <v>0.195461601811</v>
       </c>
       <c r="L24" s="1">
-        <v>-9.9450129774100005E-2</v>
+        <v>-0.13865518429699999</v>
       </c>
       <c r="M24" s="1">
-        <v>0.24192964111900001</v>
+        <v>0.202742697088</v>
       </c>
       <c r="N24" s="1">
-        <v>9.8774543403299993E-3</v>
+        <v>-9.1879710896E-2</v>
       </c>
       <c r="O24" s="1">
-        <v>0.104527505467</v>
+        <v>0.175568666007</v>
       </c>
       <c r="P24" s="1">
-        <v>0.132575614323</v>
+        <v>0.18512136646899999</v>
       </c>
       <c r="Q24" s="1">
-        <v>0.21914232212099999</v>
+        <v>0.25796827980100001</v>
       </c>
       <c r="R24" s="1">
-        <v>0.25534338225999997</v>
+        <v>0.35907555446299999</v>
       </c>
       <c r="S24" s="1">
-        <v>0.42257955717099999</v>
+        <v>0.450641862974</v>
       </c>
       <c r="T24" s="1">
-        <v>0.31955669200499998</v>
+        <v>0.34540683874900002</v>
       </c>
       <c r="U24" s="1">
-        <v>0.23848786817299999</v>
+        <v>0.30991656478000001</v>
       </c>
       <c r="V24" s="1">
-        <v>0.22299815505500001</v>
+        <v>0.303042938644</v>
       </c>
       <c r="W24" s="1">
-        <v>0.20077119923200001</v>
+        <v>0.25710976335300001</v>
       </c>
       <c r="X24" s="1">
-        <v>0.29297234287899998</v>
+        <v>0.31363873047700003</v>
       </c>
       <c r="Y24" s="1">
-        <v>0.20180408505399999</v>
+        <v>0.204933952147</v>
       </c>
       <c r="Z24" s="1">
-        <v>0.53138715776500001</v>
+        <v>0.66775812474499996</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1">
-        <v>-4.3922932951300002E-2</v>
+        <v>4.0708538595600002E-2</v>
       </c>
       <c r="C25" s="1">
-        <v>0.189989091272</v>
+        <v>0.137263541554</v>
       </c>
       <c r="D25" s="1">
-        <v>3.9868948970999997E-2</v>
+        <v>-1.25530861541E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>0.105061792652</v>
+        <v>1.0187559591199999E-2</v>
       </c>
       <c r="F25" s="1">
-        <v>0.155637219662</v>
+        <v>5.43337271819E-2</v>
       </c>
       <c r="G25" s="1">
-        <v>-9.4451829262199999E-2</v>
+        <v>6.0322280173200002E-2</v>
       </c>
       <c r="H25" s="1">
-        <v>0.26281409817899998</v>
+        <v>0.28770548238999999</v>
       </c>
       <c r="I25" s="1">
-        <v>3.4238525576100001E-3</v>
+        <v>2.5015296044899999E-3</v>
       </c>
       <c r="J25" s="1">
-        <v>0.19813795920499999</v>
+        <v>-6.8272695861100003E-3</v>
       </c>
       <c r="K25" s="1">
-        <v>0.26133318276099998</v>
+        <v>9.3098671232200003E-2</v>
       </c>
       <c r="L25" s="1">
-        <v>-8.8377439138800001E-2</v>
+        <v>6.34243017144E-2</v>
       </c>
       <c r="M25" s="1">
-        <v>0.26606878416800001</v>
+        <v>0.28082063420199999</v>
       </c>
       <c r="N25" s="1">
-        <v>1.45897276569E-2</v>
+        <v>-2.9231954077999999E-3</v>
       </c>
       <c r="O25" s="1">
-        <v>0.189282174208</v>
+        <v>-1.50081416636E-3</v>
       </c>
       <c r="P25" s="1">
-        <v>0.254717344929</v>
+        <v>9.4668588817800006E-2</v>
       </c>
       <c r="Q25" s="1">
-        <v>0.29605161783099998</v>
+        <v>0.33050073022900001</v>
       </c>
       <c r="R25" s="1">
-        <v>0.33337413213099998</v>
+        <v>0.19055990326200001</v>
       </c>
       <c r="S25" s="1">
-        <v>0.47805313856100001</v>
+        <v>0.34441990162699998</v>
       </c>
       <c r="T25" s="1">
-        <v>0.38998444216799999</v>
+        <v>0.37268274161999998</v>
       </c>
       <c r="U25" s="1">
-        <v>0.40176231948800001</v>
+        <v>0.19271740228500001</v>
       </c>
       <c r="V25" s="1">
-        <v>0.37004785445600002</v>
+        <v>0.26758386458700001</v>
       </c>
       <c r="W25" s="1">
-        <v>0.33391683234300001</v>
+        <v>0.210390565334</v>
       </c>
       <c r="X25" s="1">
-        <v>0.31379360285399999</v>
+        <v>8.0771238575100004E-2</v>
       </c>
       <c r="Y25" s="1">
-        <v>0.22758890430299999</v>
+        <v>3.9671533752399998E-2</v>
       </c>
       <c r="Z25" s="1">
-        <v>0.72572284111300001</v>
+        <v>0.493719640972</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1">
-        <v>-3.8591123996200002E-2</v>
+        <v>-4.7630537009899998E-2</v>
       </c>
       <c r="C26" s="1">
-        <v>6.95436499111E-2</v>
+        <v>0.12403377466399999</v>
       </c>
       <c r="D26" s="1">
-        <v>2.6672935653799999E-2</v>
+        <v>6.6582926381299999E-3</v>
       </c>
       <c r="E26" s="1">
-        <v>9.4378329428900006E-3</v>
+        <v>6.6993104952300001E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>6.6086232004199996E-2</v>
+        <v>6.8742972567800001E-2</v>
       </c>
       <c r="G26" s="1">
-        <v>-6.3047589717000002E-2</v>
+        <v>-9.6750189361399994E-2</v>
       </c>
       <c r="H26" s="1">
-        <v>0.12577639486799999</v>
+        <v>0.205758351162</v>
       </c>
       <c r="I26" s="1">
-        <v>-4.7452809059599997E-2</v>
+        <v>-4.7537484465099998E-2</v>
       </c>
       <c r="J26" s="1">
-        <v>3.8281179458199997E-2</v>
+        <v>7.9918579742099996E-2</v>
       </c>
       <c r="K26" s="1">
-        <v>0.113606859379</v>
+        <v>0.16189080978100001</v>
       </c>
       <c r="L26" s="1">
-        <v>-6.1788126766799997E-2</v>
+        <v>-9.4559249476599994E-2</v>
       </c>
       <c r="M26" s="1">
-        <v>0.120960158651</v>
+        <v>0.20856677357299999</v>
       </c>
       <c r="N26" s="1">
-        <v>-2.85554916131E-2</v>
+        <v>-3.6578151633400002E-2</v>
       </c>
       <c r="O26" s="1">
-        <v>3.3065579723999997E-2</v>
+        <v>8.7235464533599996E-2</v>
       </c>
       <c r="P26" s="1">
-        <v>0.11036550793699999</v>
+        <v>0.15460531138899999</v>
       </c>
       <c r="Q26" s="1">
-        <v>0.24368568859699999</v>
+        <v>0.23399070411199999</v>
       </c>
       <c r="R26" s="1">
-        <v>0.282115467718</v>
+        <v>0.25661056759299999</v>
       </c>
       <c r="S26" s="1">
-        <v>0.43097491600600002</v>
+        <v>0.38386499456599998</v>
       </c>
       <c r="T26" s="1">
-        <v>0.35065157622499998</v>
+        <v>0.34599419833099998</v>
       </c>
       <c r="U26" s="1">
-        <v>0.283873057135</v>
+        <v>0.320162659214</v>
       </c>
       <c r="V26" s="1">
-        <v>0.20880962624400001</v>
+        <v>0.204834523602</v>
       </c>
       <c r="W26" s="1">
-        <v>0.204712632295</v>
+        <v>0.19649582228199999</v>
       </c>
       <c r="X26" s="1">
-        <v>0.26190970436200001</v>
+        <v>0.22139658206099999</v>
       </c>
       <c r="Y26" s="1">
-        <v>0.20987184582599999</v>
+        <v>0.11429282187000001</v>
       </c>
       <c r="Z26" s="1">
-        <v>0.53968549546599998</v>
+        <v>0.50061972563799995</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1">
-        <v>-5.5869371492199997E-2</v>
+        <v>3.2281060828299998E-2</v>
       </c>
       <c r="C27" s="1">
-        <v>0.13171469455199999</v>
+        <v>0.118066094092</v>
       </c>
       <c r="D27" s="1">
-        <v>-9.1916054290499996E-2</v>
+        <v>-2.61392593787E-2</v>
       </c>
       <c r="E27" s="1">
-        <v>2.6702737865599999E-2</v>
+        <v>-1.9111785090699999E-2</v>
       </c>
       <c r="F27" s="1">
-        <v>6.0182381336799998E-2</v>
+        <v>5.7240431898099998E-2</v>
       </c>
       <c r="G27" s="1">
-        <v>-5.7161330941600003E-2</v>
+        <v>-4.3332770453599997E-2</v>
       </c>
       <c r="H27" s="1">
-        <v>0.22902526120700001</v>
+        <v>0.110953346105</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.106273439555</v>
+        <v>-3.5959192133200001E-2</v>
       </c>
       <c r="J27" s="1">
-        <v>2.5088852395699999E-2</v>
+        <v>2.5688419357299999E-2</v>
       </c>
       <c r="K27" s="1">
-        <v>7.1164212683700004E-2</v>
+        <v>8.9080983824200002E-2</v>
       </c>
       <c r="L27" s="1">
-        <v>-6.4503295074400002E-2</v>
+        <v>-2.3372574398200001E-2</v>
       </c>
       <c r="M27" s="1">
-        <v>0.22984879934800001</v>
+        <v>0.12483179556100001</v>
       </c>
       <c r="N27" s="1">
-        <v>-0.11620690513199999</v>
+        <v>-3.6545028697799999E-2</v>
       </c>
       <c r="O27" s="1">
-        <v>2.8986654413299999E-2</v>
+        <v>1.39513960622E-2</v>
       </c>
       <c r="P27" s="1">
-        <v>7.7411889417000002E-2</v>
+        <v>8.8098243068400001E-2</v>
       </c>
       <c r="Q27" s="1">
-        <v>0.21345489364799999</v>
+        <v>0.31262000576799998</v>
       </c>
       <c r="R27" s="1">
-        <v>0.26201130450100002</v>
+        <v>0.28923731277100001</v>
       </c>
       <c r="S27" s="1">
-        <v>0.26494998506099998</v>
+        <v>0.46189842037000001</v>
       </c>
       <c r="T27" s="1">
-        <v>0.23457903312799999</v>
+        <v>0.41103762754200002</v>
       </c>
       <c r="U27" s="1">
-        <v>0.150036602549</v>
+        <v>0.25553471360199997</v>
       </c>
       <c r="V27" s="1">
-        <v>0.14590969089899999</v>
+        <v>0.26737842477899998</v>
       </c>
       <c r="W27" s="1">
-        <v>0.138640244538</v>
+        <v>0.24036802603499999</v>
       </c>
       <c r="X27" s="1">
-        <v>0.181119234785</v>
+        <v>0.27359070037400002</v>
       </c>
       <c r="Y27" s="1">
-        <v>9.9304238517199994E-2</v>
+        <v>0.197283823286</v>
       </c>
       <c r="Z27" s="1">
-        <v>0.419374042477</v>
+        <v>0.57894027108699997</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1">
-        <v>-4.2633173179500002E-2</v>
+        <v>-3.8591123996200002E-2</v>
       </c>
       <c r="C28" s="1">
-        <v>0.130106377302</v>
+        <v>6.95436499111E-2</v>
       </c>
       <c r="D28" s="1">
-        <v>2.5137669812799999E-2</v>
+        <v>2.6672935653799999E-2</v>
       </c>
       <c r="E28" s="1">
-        <v>4.5446442639200002E-2</v>
+        <v>9.4378329428900006E-3</v>
       </c>
       <c r="F28" s="1">
-        <v>7.7129220694799994E-2</v>
+        <v>6.6086232004199996E-2</v>
       </c>
       <c r="G28" s="1">
-        <v>-6.4041473614000005E-2</v>
+        <v>-6.3047589717000002E-2</v>
       </c>
       <c r="H28" s="1">
-        <v>0.17729838513900001</v>
+        <v>0.12577639486799999</v>
       </c>
       <c r="I28" s="1">
-        <v>-3.3803982177099998E-2</v>
+        <v>-4.7452809059599997E-2</v>
       </c>
       <c r="J28" s="1">
-        <v>8.9438126303099996E-2</v>
+        <v>3.8281179458199997E-2</v>
       </c>
       <c r="K28" s="1">
-        <v>0.12873186240600001</v>
+        <v>0.113606859379</v>
       </c>
       <c r="L28" s="1">
-        <v>-6.5191396252000003E-2</v>
+        <v>-6.1788126766799997E-2</v>
       </c>
       <c r="M28" s="1">
-        <v>0.18447057124899999</v>
+        <v>0.120960158651</v>
       </c>
       <c r="N28" s="1">
-        <v>-1.8613917024000001E-2</v>
+        <v>-2.85554916131E-2</v>
       </c>
       <c r="O28" s="1">
-        <v>8.6383912286700004E-2</v>
+        <v>3.3065579723999997E-2</v>
       </c>
       <c r="P28" s="1">
-        <v>0.12819811738100001</v>
+        <v>0.11036550793699999</v>
       </c>
       <c r="Q28" s="1">
-        <v>0.26217738432999999</v>
+        <v>0.24368568859699999</v>
       </c>
       <c r="R28" s="1">
-        <v>0.32416281999699997</v>
+        <v>0.282115467718</v>
       </c>
       <c r="S28" s="1">
-        <v>0.52473489190099998</v>
+        <v>0.43097491600600002</v>
       </c>
       <c r="T28" s="1">
-        <v>0.41284975359199999</v>
+        <v>0.35065157622499998</v>
       </c>
       <c r="U28" s="1">
-        <v>0.27711152115400001</v>
+        <v>0.283873057135</v>
       </c>
       <c r="V28" s="1">
-        <v>0.278598491374</v>
+        <v>0.20880962624400001</v>
       </c>
       <c r="W28" s="1">
-        <v>0.26114514493699997</v>
+        <v>0.204712632295</v>
       </c>
       <c r="X28" s="1">
-        <v>0.32728406516800002</v>
+        <v>0.26190970436200001</v>
       </c>
       <c r="Y28" s="1">
-        <v>0.255156813742</v>
+        <v>0.20987184582599999</v>
       </c>
       <c r="Z28" s="1">
-        <v>0.59727215392999999</v>
+        <v>0.53968549546599998</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1">
-        <v>-3.6176171114899999E-2</v>
+        <v>1.48431358416E-2</v>
       </c>
       <c r="C29" s="1">
-        <v>0.10728780651600001</v>
+        <v>9.05679933134E-2</v>
       </c>
       <c r="D29" s="1">
-        <v>-8.3949064858499997E-2</v>
+        <v>-2.4282608886699999E-2</v>
       </c>
       <c r="E29" s="1">
-        <v>5.5413402297000001E-2</v>
+        <v>4.52103570154E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>8.4466064713699995E-2</v>
+        <v>5.6628249168600001E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>-5.2021159062799999E-2</v>
+        <v>-1.8472459240499998E-2</v>
       </c>
       <c r="H29" s="1">
-        <v>0.146241697453</v>
+        <v>0.19359720184500001</v>
       </c>
       <c r="I29" s="1">
-        <v>-9.8212232107199995E-2</v>
+        <v>-8.5184505789100001E-2</v>
       </c>
       <c r="J29" s="1">
-        <v>2.51132952531E-2</v>
+        <v>0.13426274342200001</v>
       </c>
       <c r="K29" s="1">
-        <v>0.11965675519299999</v>
+        <v>0.13689826648600001</v>
       </c>
       <c r="L29" s="1">
-        <v>-5.4733292934599997E-2</v>
+        <v>-9.8983861253499998E-3</v>
       </c>
       <c r="M29" s="1">
-        <v>0.15564463216400001</v>
+        <v>0.180412019397</v>
       </c>
       <c r="N29" s="1">
-        <v>-0.108540128007</v>
+        <v>-7.4543514194199995E-2</v>
       </c>
       <c r="O29" s="1">
-        <v>3.9081165472699998E-2</v>
+        <v>0.119739416936</v>
       </c>
       <c r="P29" s="1">
-        <v>0.126251244766</v>
+        <v>0.12529827050600001</v>
       </c>
       <c r="Q29" s="1">
-        <v>0.18892738009500001</v>
+        <v>0.408899182842</v>
       </c>
       <c r="R29" s="1">
-        <v>0.165295041951</v>
+        <v>0.37218165518099999</v>
       </c>
       <c r="S29" s="1">
-        <v>0.165122885054</v>
+        <v>0.61590521145699995</v>
       </c>
       <c r="T29" s="1">
-        <v>0.14155111829899999</v>
+        <v>0.52396003786500001</v>
       </c>
       <c r="U29" s="1">
-        <v>8.7800260714500006E-2</v>
+        <v>0.265712036373</v>
       </c>
       <c r="V29" s="1">
-        <v>6.5329074720800004E-2</v>
+        <v>0.44608898122399998</v>
       </c>
       <c r="W29" s="1">
-        <v>6.6682475135199995E-2</v>
+        <v>0.375226589326</v>
       </c>
       <c r="X29" s="1">
-        <v>8.6708632174599995E-2</v>
+        <v>0.36440152265600001</v>
       </c>
       <c r="Y29" s="1">
-        <v>5.1881835328299996E-3</v>
+        <v>0.27139960262700003</v>
       </c>
       <c r="Z29" s="1">
-        <v>0.32156897142399998</v>
+        <v>0.70784472000300003</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1">
-        <v>-6.3589077384599998E-2</v>
+        <v>-6.0443076936199998E-2</v>
       </c>
       <c r="C30" s="1">
-        <v>0.14433746606600001</v>
+        <v>0.13447018481799999</v>
       </c>
       <c r="D30" s="1">
-        <v>6.8918933092099996E-2</v>
+        <v>3.4876068761400002E-2</v>
       </c>
       <c r="E30" s="1">
-        <v>5.4798408131699998E-2</v>
+        <v>6.2718460290299996E-2</v>
       </c>
       <c r="F30" s="1">
-        <v>7.4253012043399999E-2</v>
+        <v>8.4307893024599997E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>-0.14340111166399999</v>
+        <v>-9.3120268845800006E-2</v>
       </c>
       <c r="H30" s="1">
-        <v>0.19022263852099999</v>
+        <v>0.21028877804000001</v>
       </c>
       <c r="I30" s="1">
-        <v>-0.13699852162000001</v>
+        <v>-8.6834126329499994E-2</v>
       </c>
       <c r="J30" s="1">
-        <v>0.19128508995499999</v>
+        <v>0.117960776074</v>
       </c>
       <c r="K30" s="1">
-        <v>0.195461601811</v>
+        <v>0.15854403560899999</v>
       </c>
       <c r="L30" s="1">
-        <v>-0.13865518429699999</v>
+        <v>-9.3913483912099999E-2</v>
       </c>
       <c r="M30" s="1">
-        <v>0.202742697088</v>
+        <v>0.21147128200099999</v>
       </c>
       <c r="N30" s="1">
-        <v>-9.1879710896E-2</v>
+        <v>-6.0982612889600003E-2</v>
       </c>
       <c r="O30" s="1">
-        <v>0.175568666007</v>
+        <v>0.11491277131700001</v>
       </c>
       <c r="P30" s="1">
-        <v>0.18512136646899999</v>
+        <v>0.15444407948399999</v>
       </c>
       <c r="Q30" s="1">
-        <v>0.25796827980100001</v>
+        <v>0.22651795506799999</v>
       </c>
       <c r="R30" s="1">
-        <v>0.35907555446299999</v>
+        <v>0.29090942033799999</v>
       </c>
       <c r="S30" s="1">
-        <v>0.450641862974</v>
+        <v>0.434274155188</v>
       </c>
       <c r="T30" s="1">
-        <v>0.34540683874900002</v>
+        <v>0.35069108585100001</v>
       </c>
       <c r="U30" s="1">
-        <v>0.30991656478000001</v>
+        <v>0.233008844902</v>
       </c>
       <c r="V30" s="1">
-        <v>0.303042938644</v>
+        <v>0.24755359811700001</v>
       </c>
       <c r="W30" s="1">
-        <v>0.25710976335300001</v>
+        <v>0.21563629644499999</v>
       </c>
       <c r="X30" s="1">
-        <v>0.31363873047700003</v>
+        <v>0.27600039900399997</v>
       </c>
       <c r="Y30" s="1">
-        <v>0.204933952147</v>
+        <v>0.21248613290599999</v>
       </c>
       <c r="Z30" s="1">
-        <v>0.66775812474499996</v>
+        <v>0.55733293480000001</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
-        <v>1.27972393349E-2</v>
+        <v>-1.6488118265000001E-2</v>
       </c>
       <c r="C31" s="1">
-        <v>9.9333435595899994E-2</v>
+        <v>0.12824485100999999</v>
       </c>
       <c r="D31" s="1">
-        <v>-1.5648423933800001E-2</v>
+        <v>1.94722571752E-2</v>
       </c>
       <c r="E31" s="1">
-        <v>2.1493241997999998E-2</v>
+        <v>9.4210363172200003E-4</v>
       </c>
       <c r="F31" s="1">
-        <v>5.3213139227699997E-2</v>
+        <v>2.1331906877000002E-2</v>
       </c>
       <c r="G31" s="1">
-        <v>-4.3124910792200002E-2</v>
+        <v>-3.2147694003500003E-2</v>
       </c>
       <c r="H31" s="1">
-        <v>0.12008654291199999</v>
+        <v>0.14252024866900001</v>
       </c>
       <c r="I31" s="1">
-        <v>-7.9527338331700004E-2</v>
+        <v>-1.37270839432E-2</v>
       </c>
       <c r="J31" s="1">
-        <v>6.9338786579E-2</v>
+        <v>5.92524992257E-2</v>
       </c>
       <c r="K31" s="1">
-        <v>0.143377317941</v>
+        <v>0.10288872969600001</v>
       </c>
       <c r="L31" s="1">
-        <v>-2.9416180581000002E-2</v>
+        <v>-3.0763978085000001E-2</v>
       </c>
       <c r="M31" s="1">
-        <v>0.124035076821</v>
+        <v>0.15512527306599999</v>
       </c>
       <c r="N31" s="1">
-        <v>-6.6539185139999998E-2</v>
+        <v>-4.2635512214599996E-3</v>
       </c>
       <c r="O31" s="1">
-        <v>6.0526389963199999E-2</v>
+        <v>4.7001999631399997E-2</v>
       </c>
       <c r="P31" s="1">
-        <v>0.12776758022000001</v>
+        <v>8.8182935352999994E-2</v>
       </c>
       <c r="Q31" s="1">
-        <v>0.33767250296399998</v>
+        <v>0.38160384716099999</v>
       </c>
       <c r="R31" s="1">
-        <v>0.34339401394300001</v>
+        <v>0.30157705440600002</v>
       </c>
       <c r="S31" s="1">
-        <v>0.54630395941599996</v>
+        <v>0.57467237850700004</v>
       </c>
       <c r="T31" s="1">
-        <v>0.47106685096299999</v>
+        <v>0.47418522168799998</v>
       </c>
       <c r="U31" s="1">
-        <v>0.24219110854199999</v>
+        <v>0.16967615769700001</v>
       </c>
       <c r="V31" s="1">
-        <v>0.39241549722199998</v>
+        <v>0.41118033285799999</v>
       </c>
       <c r="W31" s="1">
-        <v>0.35410415531200001</v>
+        <v>0.312564122868</v>
       </c>
       <c r="X31" s="1">
-        <v>0.32469050368300001</v>
+        <v>0.37864981797800001</v>
       </c>
       <c r="Y31" s="1">
-        <v>0.23347305674800001</v>
+        <v>0.27623693485599998</v>
       </c>
       <c r="Z31" s="1">
-        <v>0.68311253797799998</v>
+        <v>0.65480164503000005</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1">
-        <v>-5.65811451592E-2</v>
+        <v>-4.2633173179500002E-2</v>
       </c>
       <c r="C32" s="1">
-        <v>8.2523404454699995E-2</v>
+        <v>0.130106377302</v>
       </c>
       <c r="D32" s="1">
-        <v>-0.107180939446</v>
+        <v>2.5137669812799999E-2</v>
       </c>
       <c r="E32" s="1">
-        <v>1.5853974583500002E-2</v>
+        <v>4.5446442639200002E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>0.129297297093</v>
+        <v>7.7129220694799994E-2</v>
       </c>
       <c r="G32" s="1">
-        <v>-8.2474190042500006E-2</v>
+        <v>-6.4041473614000005E-2</v>
       </c>
       <c r="H32" s="1">
-        <v>0.13982330652399999</v>
+        <v>0.17729838513900001</v>
       </c>
       <c r="I32" s="1">
-        <v>-0.17548806334</v>
+        <v>-3.3803982177099998E-2</v>
       </c>
       <c r="J32" s="1">
-        <v>2.78728074035E-2</v>
+        <v>8.9438126303099996E-2</v>
       </c>
       <c r="K32" s="1">
-        <v>0.184084712663</v>
+        <v>0.12873186240600001</v>
       </c>
       <c r="L32" s="1">
-        <v>-8.5534685890800002E-2</v>
+        <v>-6.5191396252000003E-2</v>
       </c>
       <c r="M32" s="1">
-        <v>0.141123880688</v>
+        <v>0.18447057124899999</v>
       </c>
       <c r="N32" s="1">
-        <v>-0.178184516264</v>
+        <v>-1.8613917024000001E-2</v>
       </c>
       <c r="O32" s="1">
-        <v>2.8005992409100001E-2</v>
+        <v>8.6383912286700004E-2</v>
       </c>
       <c r="P32" s="1">
-        <v>0.19181706549899999</v>
+        <v>0.12819811738100001</v>
       </c>
       <c r="Q32" s="1">
-        <v>0.19124211172899999</v>
+        <v>0.26217738432999999</v>
       </c>
       <c r="R32" s="1">
-        <v>0.15516921735799999</v>
+        <v>0.32416281999699997</v>
       </c>
       <c r="S32" s="1">
-        <v>0.22082391967199999</v>
+        <v>0.52473489190099998</v>
       </c>
       <c r="T32" s="1">
-        <v>0.18553876906299999</v>
+        <v>0.41284975359199999</v>
       </c>
       <c r="U32" s="1">
-        <v>9.8063302964099999E-2</v>
+        <v>0.27711152115400001</v>
       </c>
       <c r="V32" s="1">
-        <v>0.104259113027</v>
+        <v>0.278598491374</v>
       </c>
       <c r="W32" s="1">
-        <v>0.103927754085</v>
+        <v>0.26114514493699997</v>
       </c>
       <c r="X32" s="1">
-        <v>0.115917879712</v>
+        <v>0.32728406516800002</v>
       </c>
       <c r="Y32" s="1">
-        <v>-4.5541788022599996E-3</v>
+        <v>0.255156813742</v>
       </c>
       <c r="Z32" s="1">
-        <v>0.36803728026100002</v>
+        <v>0.59727215392999999</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
-        <v>-8.6846705604399999E-2</v>
+        <v>-7.4633277030100004E-2</v>
       </c>
       <c r="C33" s="1">
-        <v>8.9134465684999997E-2</v>
+        <v>0.19075293416899999</v>
       </c>
       <c r="D33" s="1">
-        <v>4.25647507299E-2</v>
+        <v>4.5293908728600001E-2</v>
       </c>
       <c r="E33" s="1">
-        <v>-2.3613114355399999E-2</v>
+        <v>8.2179955708499994E-2</v>
       </c>
       <c r="F33" s="1">
-        <v>6.7713552056899995E-2</v>
+        <v>0.106061164528</v>
       </c>
       <c r="G33" s="1">
-        <v>-0.109236455607</v>
+        <v>-0.103373911225</v>
       </c>
       <c r="H33" s="1">
-        <v>0.17214113169100001</v>
+        <v>0.22862546036100001</v>
       </c>
       <c r="I33" s="1">
-        <v>3.17895646638E-2</v>
+        <v>-1.28923038541E-2</v>
       </c>
       <c r="J33" s="1">
-        <v>-2.80541963615E-2</v>
+        <v>0.13563843952999999</v>
       </c>
       <c r="K33" s="1">
-        <v>0.122676288038</v>
+        <v>0.170629249407</v>
       </c>
       <c r="L33" s="1">
-        <v>-0.114933318366</v>
+        <v>-0.10708642817400001</v>
       </c>
       <c r="M33" s="1">
-        <v>0.16709433291199999</v>
+        <v>0.245022854811</v>
       </c>
       <c r="N33" s="1">
-        <v>3.8543227091100002E-2</v>
+        <v>3.9759334268099997E-3</v>
       </c>
       <c r="O33" s="1">
-        <v>-2.9912703459899999E-2</v>
+        <v>0.13555231832100001</v>
       </c>
       <c r="P33" s="1">
-        <v>0.12030488244900001</v>
+        <v>0.17138108756699999</v>
       </c>
       <c r="Q33" s="1">
-        <v>0.20843667672300001</v>
+        <v>0.211925832157</v>
       </c>
       <c r="R33" s="1">
-        <v>0.32185713847199998</v>
+        <v>0.235376190234</v>
       </c>
       <c r="S33" s="1">
-        <v>0.38309032618599997</v>
+        <v>0.36583828063000001</v>
       </c>
       <c r="T33" s="1">
-        <v>0.32068007554799999</v>
+        <v>0.29309070420700001</v>
       </c>
       <c r="U33" s="1">
-        <v>0.33377998523000002</v>
+        <v>0.25458062889299998</v>
       </c>
       <c r="V33" s="1">
-        <v>0.16455676681199999</v>
+        <v>0.20777078356199999</v>
       </c>
       <c r="W33" s="1">
-        <v>0.20615404232500001</v>
+        <v>0.182330782469</v>
       </c>
       <c r="X33" s="1">
-        <v>0.27703664256799998</v>
+        <v>0.222273511191</v>
       </c>
       <c r="Y33" s="1">
-        <v>0.25353907007600002</v>
+        <v>0.16699306143199999</v>
       </c>
       <c r="Z33" s="1">
-        <v>0.46753328669100003</v>
+        <v>0.49504912022699998</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1">
-        <v>-4.6372790671099999E-2</v>
+        <v>-6.7358902629599995E-2</v>
       </c>
       <c r="C34" s="1">
-        <v>0.105107739573</v>
+        <v>0.158632512856</v>
       </c>
       <c r="D34" s="1">
-        <v>8.9663216075799995E-2</v>
+        <v>3.3797436588600002E-2</v>
       </c>
       <c r="E34" s="1">
-        <v>3.1318679213099998E-2</v>
+        <v>6.0146720432199999E-2</v>
       </c>
       <c r="F34" s="1">
-        <v>5.5299083474399997E-2</v>
+        <v>8.9313858498100002E-2</v>
       </c>
       <c r="G34" s="1">
-        <v>-7.81717137044E-2</v>
+        <v>-9.6386326904099998E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>0.173299951678</v>
+        <v>0.23630622872599999</v>
       </c>
       <c r="I34" s="1">
-        <v>2.0397148847700001E-2</v>
+        <v>-4.0791023134399999E-4</v>
       </c>
       <c r="J34" s="1">
-        <v>6.7742063634399996E-2</v>
+        <v>0.105186071827</v>
       </c>
       <c r="K34" s="1">
-        <v>0.12808641482800001</v>
+        <v>0.128614743192</v>
       </c>
       <c r="L34" s="1">
-        <v>-7.9141985035199994E-2</v>
+        <v>-9.9450129774100005E-2</v>
       </c>
       <c r="M34" s="1">
-        <v>0.176268572845</v>
+        <v>0.24192964111900001</v>
       </c>
       <c r="N34" s="1">
-        <v>4.76102430001E-2</v>
+        <v>9.8774543403299993E-3</v>
       </c>
       <c r="O34" s="1">
-        <v>6.5538129019700006E-2</v>
+        <v>0.104527505467</v>
       </c>
       <c r="P34" s="1">
-        <v>0.12255186945800001</v>
+        <v>0.132575614323</v>
       </c>
       <c r="Q34" s="1">
-        <v>0.29136061799899998</v>
+        <v>0.21914232212099999</v>
       </c>
       <c r="R34" s="1">
-        <v>0.31193789193499999</v>
+        <v>0.25534338225999997</v>
       </c>
       <c r="S34" s="1">
-        <v>0.37002628786800001</v>
+        <v>0.42257955717099999</v>
       </c>
       <c r="T34" s="1">
-        <v>0.33330018090899999</v>
+        <v>0.31955669200499998</v>
       </c>
       <c r="U34" s="1">
-        <v>0.258453465321</v>
+        <v>0.23848786817299999</v>
       </c>
       <c r="V34" s="1">
-        <v>0.227404279322</v>
+        <v>0.22299815505500001</v>
       </c>
       <c r="W34" s="1">
-        <v>0.25844536292499998</v>
+        <v>0.20077119923200001</v>
       </c>
       <c r="X34" s="1">
-        <v>0.289870286202</v>
+        <v>0.29297234287899998</v>
       </c>
       <c r="Y34" s="1">
-        <v>0.22116053271200001</v>
+        <v>0.20180408505399999</v>
       </c>
       <c r="Z34" s="1">
-        <v>0.52623426729900002</v>
+        <v>0.53138715776500001</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1">
-        <v>-3.5817667495400003E-2</v>
+        <v>-1.09083309484E-2</v>
       </c>
       <c r="C35" s="1">
-        <v>9.1584697625299999E-2</v>
+        <v>0.118672971471</v>
       </c>
       <c r="D35" s="1">
-        <v>2.09327344025E-2</v>
+        <v>-5.61368380409E-2</v>
       </c>
       <c r="E35" s="1">
-        <v>6.1858432602200003E-2</v>
+        <v>2.2890257526100001E-2</v>
       </c>
       <c r="F35" s="1">
-        <v>4.7959149726899998E-2</v>
+        <v>5.9445982753399997E-2</v>
       </c>
       <c r="G35" s="1">
-        <v>-3.2953119695799997E-2</v>
+        <v>-7.1570202221200002E-2</v>
       </c>
       <c r="H35" s="1">
-        <v>0.161962734783</v>
+        <v>0.148872710278</v>
       </c>
       <c r="I35" s="1">
-        <v>8.0787710002399996E-4</v>
+        <v>-0.16590471968100001</v>
       </c>
       <c r="J35" s="1">
-        <v>6.6172815304599994E-2</v>
+        <v>0.123954220107</v>
       </c>
       <c r="K35" s="1">
-        <v>7.6294283020599998E-2</v>
+        <v>0.249296340842</v>
       </c>
       <c r="L35" s="1">
-        <v>-3.9443477882199998E-2</v>
+        <v>-6.23842340107E-2</v>
       </c>
       <c r="M35" s="1">
-        <v>0.165228532613</v>
+        <v>0.16079054240000001</v>
       </c>
       <c r="N35" s="1">
-        <v>7.7846250252499999E-3</v>
+        <v>-0.15478846458600001</v>
       </c>
       <c r="O35" s="1">
-        <v>7.5836054328800001E-2</v>
+        <v>0.109481322536</v>
       </c>
       <c r="P35" s="1">
-        <v>7.9448567880199994E-2</v>
+        <v>0.22452566828600001</v>
       </c>
       <c r="Q35" s="1">
-        <v>0.36031233327700002</v>
+        <v>0.30078462464099998</v>
       </c>
       <c r="R35" s="1">
-        <v>0.43906338901899999</v>
+        <v>0.16353138871600001</v>
       </c>
       <c r="S35" s="1">
-        <v>0.427419992473</v>
+        <v>0.39526428822800003</v>
       </c>
       <c r="T35" s="1">
-        <v>0.41378428965199998</v>
+        <v>0.364081629666</v>
       </c>
       <c r="U35" s="1">
-        <v>0.39720121516200002</v>
+        <v>0.23694572435700001</v>
       </c>
       <c r="V35" s="1">
-        <v>0.267081134346</v>
+        <v>0.27872489824699997</v>
       </c>
       <c r="W35" s="1">
-        <v>0.22497140585100001</v>
+        <v>0.279544464208</v>
       </c>
       <c r="X35" s="1">
-        <v>0.383650878902</v>
+        <v>0.20423316539</v>
       </c>
       <c r="Y35" s="1">
-        <v>0.36304065129300001</v>
+        <v>4.3476312601499999E-2</v>
       </c>
       <c r="Z35" s="1">
-        <v>0.51636992098800005</v>
+        <v>0.49263589198500002</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>-3.3872842694200003E-2</v>
+        <v>-7.0660464790199995E-2</v>
       </c>
       <c r="C36" s="1">
-        <v>0.104811256162</v>
+        <v>0.12566336856400001</v>
       </c>
       <c r="D36" s="1">
-        <v>-8.40042587511E-2</v>
+        <v>7.2595324421000001E-2</v>
       </c>
       <c r="E36" s="1">
-        <v>3.8097180386100001E-2</v>
+        <v>4.6339745626699999E-2</v>
       </c>
       <c r="F36" s="1">
-        <v>7.3828947253100005E-2</v>
+        <v>8.2484244205699997E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>-9.8635019504299995E-2</v>
+        <v>-8.6749093793699994E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>0.19255424566900001</v>
+        <v>0.184475696243</v>
       </c>
       <c r="I36" s="1">
-        <v>-0.207937538353</v>
+        <v>-5.1531225685099998E-2</v>
       </c>
       <c r="J36" s="1">
-        <v>2.39205209842E-2</v>
+        <v>1.7704089823100001E-2</v>
       </c>
       <c r="K36" s="1">
-        <v>0.15360217407000001</v>
+        <v>0.11516116481200001</v>
       </c>
       <c r="L36" s="1">
-        <v>-9.3229561929400004E-2</v>
+        <v>-9.8021595182299998E-2</v>
       </c>
       <c r="M36" s="1">
-        <v>0.19447959614099999</v>
+        <v>0.198394222753</v>
       </c>
       <c r="N36" s="1">
-        <v>-0.200603692088</v>
+        <v>-1.14321233914E-2</v>
       </c>
       <c r="O36" s="1">
-        <v>3.2257824113000003E-2</v>
+        <v>3.3050494043900001E-2</v>
       </c>
       <c r="P36" s="1">
-        <v>0.15199987561700001</v>
+        <v>0.12544949335</v>
       </c>
       <c r="Q36" s="1">
-        <v>0.22082916900499999</v>
+        <v>0.22444607568300001</v>
       </c>
       <c r="R36" s="1">
-        <v>0.25978083088199999</v>
+        <v>0.29189506039000002</v>
       </c>
       <c r="S36" s="1">
-        <v>0.25589919743700001</v>
+        <v>0.38698686446300001</v>
       </c>
       <c r="T36" s="1">
-        <v>0.22894832336400001</v>
+        <v>0.33792513483300002</v>
       </c>
       <c r="U36" s="1">
-        <v>0.12292803222699999</v>
+        <v>0.33158414439599998</v>
       </c>
       <c r="V36" s="1">
-        <v>0.15551247132000001</v>
+        <v>0.20622455451300001</v>
       </c>
       <c r="W36" s="1">
-        <v>0.151278967254</v>
+        <v>0.20996610400900001</v>
       </c>
       <c r="X36" s="1">
-        <v>0.137623573818</v>
+        <v>0.28404384470799998</v>
       </c>
       <c r="Y36" s="1">
-        <v>5.2483237512700003E-2</v>
+        <v>0.21347702421299999</v>
       </c>
       <c r="Z36" s="1">
-        <v>0.38974621171200002</v>
+        <v>0.49443470395299999</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1">
-        <v>-3.3302422801299997E-2</v>
+        <v>-4.6372790671099999E-2</v>
       </c>
       <c r="C37" s="1">
-        <v>8.6861373600399999E-2</v>
+        <v>0.105107739573</v>
       </c>
       <c r="D37" s="1">
-        <v>2.9046540744699999E-2</v>
+        <v>8.9663216075799995E-2</v>
       </c>
       <c r="E37" s="1">
-        <v>3.6301700266399999E-2</v>
+        <v>3.1318679213099998E-2</v>
       </c>
       <c r="F37" s="1">
-        <v>8.2655199688699998E-2</v>
+        <v>5.5299083474399997E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>-3.5930478955100001E-2</v>
+        <v>-7.81717137044E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>6.8239982293800003E-2</v>
+        <v>0.173299951678</v>
       </c>
       <c r="I37" s="1">
-        <v>-2.3049542138599999E-2</v>
+        <v>2.0397148847700001E-2</v>
       </c>
       <c r="J37" s="1">
-        <v>8.2964506431400006E-2</v>
+        <v>6.7742063634399996E-2</v>
       </c>
       <c r="K37" s="1">
-        <v>0.125971475601</v>
+        <v>0.12808641482800001</v>
       </c>
       <c r="L37" s="1">
-        <v>-3.9506330672499999E-2</v>
+        <v>-7.9141985035199994E-2</v>
       </c>
       <c r="M37" s="1">
-        <v>8.2444070325099997E-2</v>
+        <v>0.176268572845</v>
       </c>
       <c r="N37" s="1">
-        <v>-9.3914956343799996E-3</v>
+        <v>4.76102430001E-2</v>
       </c>
       <c r="O37" s="1">
-        <v>7.8364702307199996E-2</v>
+        <v>6.5538129019700006E-2</v>
       </c>
       <c r="P37" s="1">
-        <v>0.12767762411799999</v>
+        <v>0.12255186945800001</v>
       </c>
       <c r="Q37" s="1">
-        <v>0.29325302344999998</v>
+        <v>0.29136061799899998</v>
       </c>
       <c r="R37" s="1">
-        <v>0.27513555389900002</v>
+        <v>0.31193789193499999</v>
       </c>
       <c r="S37" s="1">
-        <v>0.40288890958099999</v>
+        <v>0.37002628786800001</v>
       </c>
       <c r="T37" s="1">
-        <v>0.35103522250899999</v>
+        <v>0.33330018090899999</v>
       </c>
       <c r="U37" s="1">
-        <v>0.23123224673699999</v>
+        <v>0.258453465321</v>
       </c>
       <c r="V37" s="1">
-        <v>0.17957949252700001</v>
+        <v>0.227404279322</v>
       </c>
       <c r="W37" s="1">
-        <v>0.177467437935</v>
+        <v>0.25844536292499998</v>
       </c>
       <c r="X37" s="1">
-        <v>0.26321637234700002</v>
+        <v>0.289870286202</v>
       </c>
       <c r="Y37" s="1">
-        <v>0.21133263341299999</v>
+        <v>0.22116053271200001</v>
       </c>
       <c r="Z37" s="1">
-        <v>0.54110912574299996</v>
+        <v>0.52623426729900002</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1">
-        <v>-1.09083309484E-2</v>
+        <v>-6.76086737828E-2</v>
       </c>
       <c r="C38" s="1">
-        <v>0.118672971471</v>
+        <v>0.14843505356600001</v>
       </c>
       <c r="D38" s="1">
-        <v>-5.61368380409E-2</v>
+        <v>4.5954649673699999E-2</v>
       </c>
       <c r="E38" s="1">
-        <v>2.2890257526100001E-2</v>
+        <v>3.1920558242599997E-2</v>
       </c>
       <c r="F38" s="1">
-        <v>5.9445982753399997E-2</v>
+        <v>7.49519943593E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>-7.1570202221200002E-2</v>
+        <v>-7.26263423297E-2</v>
       </c>
       <c r="H38" s="1">
-        <v>0.148872710278</v>
+        <v>0.17143772037300001</v>
       </c>
       <c r="I38" s="1">
-        <v>-0.16590471968100001</v>
+        <v>4.2530759383699997E-2</v>
       </c>
       <c r="J38" s="1">
-        <v>0.123954220107</v>
+        <v>5.0308750919099997E-2</v>
       </c>
       <c r="K38" s="1">
-        <v>0.249296340842</v>
+        <v>0.105029377356</v>
       </c>
       <c r="L38" s="1">
-        <v>-6.23842340107E-2</v>
+        <v>-7.8916660431900001E-2</v>
       </c>
       <c r="M38" s="1">
-        <v>0.16079054240000001</v>
+        <v>0.183122339602</v>
       </c>
       <c r="N38" s="1">
-        <v>-0.15478846458600001</v>
+        <v>4.8038438070200001E-2</v>
       </c>
       <c r="O38" s="1">
-        <v>0.109481322536</v>
+        <v>5.04017363798E-2</v>
       </c>
       <c r="P38" s="1">
-        <v>0.22452566828600001</v>
+        <v>0.107607552573</v>
       </c>
       <c r="Q38" s="1">
-        <v>0.30078462464099998</v>
+        <v>0.23236048588700001</v>
       </c>
       <c r="R38" s="1">
-        <v>0.16353138871600001</v>
+        <v>0.24911849977799999</v>
       </c>
       <c r="S38" s="1">
-        <v>0.39526428822800003</v>
+        <v>0.382882621619</v>
       </c>
       <c r="T38" s="1">
-        <v>0.364081629666</v>
+        <v>0.30228495523799997</v>
       </c>
       <c r="U38" s="1">
-        <v>0.23694572435700001</v>
+        <v>0.242510769268</v>
       </c>
       <c r="V38" s="1">
-        <v>0.27872489824699997</v>
+        <v>0.17856697654000001</v>
       </c>
       <c r="W38" s="1">
-        <v>0.279544464208</v>
+        <v>0.17536646074000001</v>
       </c>
       <c r="X38" s="1">
-        <v>0.20423316539</v>
+        <v>0.25437057344000003</v>
       </c>
       <c r="Y38" s="1">
-        <v>4.3476312601499999E-2</v>
+        <v>0.21916875651600001</v>
       </c>
       <c r="Z38" s="1">
-        <v>0.49263589198500002</v>
+        <v>0.49941279846100001</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1">
-        <v>7.7053541672200002E-3</v>
+        <v>4.4783031349100002E-3</v>
       </c>
       <c r="C39" s="1">
-        <v>0.120196039455</v>
+        <v>5.4601585995E-2</v>
       </c>
       <c r="D39" s="1">
-        <v>3.52187458792E-2</v>
+        <v>-7.0926180637200006E-2</v>
       </c>
       <c r="E39" s="1">
-        <v>6.6310229242199994E-2</v>
+        <v>8.6756108227100004E-2</v>
       </c>
       <c r="F39" s="1">
-        <v>7.1202294633500002E-2</v>
+        <v>9.6336832912900003E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>-6.8715119662299998E-2</v>
+        <v>-6.5315451201999997E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>0.1524926285</v>
+        <v>0.14526082011700001</v>
       </c>
       <c r="I39" s="1">
-        <v>-8.0050303628199995E-2</v>
+        <v>-0.20107058605600001</v>
       </c>
       <c r="J39" s="1">
-        <v>8.2899162823500003E-2</v>
+        <v>7.2294579929E-2</v>
       </c>
       <c r="K39" s="1">
-        <v>0.10910674658</v>
+        <v>0.205817779969</v>
       </c>
       <c r="L39" s="1">
-        <v>-5.0557829489599998E-2</v>
+        <v>-5.3984817593900003E-2</v>
       </c>
       <c r="M39" s="1">
-        <v>0.156583205364</v>
+        <v>0.14205782136699999</v>
       </c>
       <c r="N39" s="1">
-        <v>-5.0432100855099998E-2</v>
+        <v>-0.19506845812900001</v>
       </c>
       <c r="O39" s="1">
-        <v>8.5473089467700006E-2</v>
+        <v>9.0999780303599995E-2</v>
       </c>
       <c r="P39" s="1">
-        <v>0.10723352139099999</v>
+        <v>0.20779353945199999</v>
       </c>
       <c r="Q39" s="1">
-        <v>0.342694078618</v>
+        <v>0.247325665995</v>
       </c>
       <c r="R39" s="1">
-        <v>0.44199682184200001</v>
+        <v>0.20020441309000001</v>
       </c>
       <c r="S39" s="1">
-        <v>0.54225003558700002</v>
+        <v>0.30872375891100001</v>
       </c>
       <c r="T39" s="1">
-        <v>0.45334718392599999</v>
+        <v>0.26368900328900002</v>
       </c>
       <c r="U39" s="1">
-        <v>0.311521109676</v>
+        <v>0.16906732767999999</v>
       </c>
       <c r="V39" s="1">
-        <v>0.37484667082299999</v>
+        <v>0.153381042286</v>
       </c>
       <c r="W39" s="1">
-        <v>0.34492040409899999</v>
+        <v>0.138265934275</v>
       </c>
       <c r="X39" s="1">
-        <v>0.42129306594799998</v>
+        <v>0.119249770385</v>
       </c>
       <c r="Y39" s="1">
-        <v>0.32149819761499998</v>
+        <v>-3.6742809052899998E-2</v>
       </c>
       <c r="Z39" s="1">
-        <v>0.65791709763100004</v>
+        <v>0.38313293113199998</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
-        <v>-2.13531752727E-2</v>
+        <v>-6.9100301815299997E-2</v>
       </c>
       <c r="C40" s="1">
-        <v>0.101551492715</v>
+        <v>0.10345943905</v>
       </c>
       <c r="D40" s="1">
-        <v>-9.52045242066E-2</v>
+        <v>-1.0571937721099999E-2</v>
       </c>
       <c r="E40" s="1">
-        <v>4.5497156405699998E-2</v>
+        <v>6.9122577524000001E-2</v>
       </c>
       <c r="F40" s="1">
-        <v>7.4726358121200001E-2</v>
+        <v>0.100349349404</v>
       </c>
       <c r="G40" s="1">
-        <v>-7.3107431933899999E-2</v>
+        <v>-0.105268807016</v>
       </c>
       <c r="H40" s="1">
-        <v>0.15898512776400001</v>
+        <v>0.18209078874699999</v>
       </c>
       <c r="I40" s="1">
-        <v>-0.22014427673199999</v>
+        <v>-0.104644736303</v>
       </c>
       <c r="J40" s="1">
-        <v>2.2170921381500001E-2</v>
+        <v>4.9527271412299997E-2</v>
       </c>
       <c r="K40" s="1">
-        <v>0.18040040163599999</v>
+        <v>0.17445594262700001</v>
       </c>
       <c r="L40" s="1">
-        <v>-6.8130322106099997E-2</v>
+        <v>-0.109255149339</v>
       </c>
       <c r="M40" s="1">
-        <v>0.16726742536299999</v>
+        <v>0.18358123360699999</v>
       </c>
       <c r="N40" s="1">
-        <v>-0.21586471172999999</v>
+        <v>-8.9094310606300006E-2</v>
       </c>
       <c r="O40" s="1">
-        <v>3.4117413798999997E-2</v>
+        <v>6.3725723678699997E-2</v>
       </c>
       <c r="P40" s="1">
-        <v>0.17577134414199999</v>
+        <v>0.17626849044699999</v>
       </c>
       <c r="Q40" s="1">
-        <v>0.19849261846899999</v>
+        <v>0.217924747344</v>
       </c>
       <c r="R40" s="1">
-        <v>0.21668326603499999</v>
+        <v>0.22376549667599999</v>
       </c>
       <c r="S40" s="1">
-        <v>0.19207543757000001</v>
+        <v>0.357145373993</v>
       </c>
       <c r="T40" s="1">
-        <v>0.168375355039</v>
+        <v>0.31932297472900001</v>
       </c>
       <c r="U40" s="1">
-        <v>0.125638752982</v>
+        <v>0.29636668298199997</v>
       </c>
       <c r="V40" s="1">
-        <v>0.14149919411699999</v>
+        <v>0.19405140334500001</v>
       </c>
       <c r="W40" s="1">
-        <v>0.12434125518</v>
+        <v>0.19759564192599999</v>
       </c>
       <c r="X40" s="1">
-        <v>0.106772231774</v>
+        <v>0.20434790579000001</v>
       </c>
       <c r="Y40" s="1">
-        <v>-4.3429612474300001E-2</v>
+        <v>9.5538906489600006E-2</v>
       </c>
       <c r="Z40" s="1">
-        <v>0.32710994249600001</v>
+        <v>0.45569815251000001</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1">
-        <v>-7.4193326688300004E-2</v>
+        <v>-3.2801876895500001E-2</v>
       </c>
       <c r="C41" s="1">
-        <v>0.113293110041</v>
+        <v>6.2564003163799994E-2</v>
       </c>
       <c r="D41" s="1">
-        <v>-4.2755590377600003E-2</v>
+        <v>9.78841048055E-3</v>
       </c>
       <c r="E41" s="1">
-        <v>2.8467863691299999E-2</v>
+        <v>6.7907279451699998E-2</v>
       </c>
       <c r="F41" s="1">
-        <v>0.10498836508499999</v>
+        <v>7.4973650728200003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>-0.101570881502</v>
+        <v>-7.9994533267600004E-2</v>
       </c>
       <c r="H41" s="1">
-        <v>0.15932009120999999</v>
+        <v>0.145783034901</v>
       </c>
       <c r="I41" s="1">
-        <v>-0.112442700163</v>
+        <v>4.1810599625E-2</v>
       </c>
       <c r="J41" s="1">
-        <v>4.0342681979199997E-2</v>
+        <v>2.9822947080400002E-2</v>
       </c>
       <c r="K41" s="1">
-        <v>0.143737848384</v>
+        <v>9.7750612035000004E-2</v>
       </c>
       <c r="L41" s="1">
-        <v>-0.105165378441</v>
+        <v>-7.7336395777899997E-2</v>
       </c>
       <c r="M41" s="1">
-        <v>0.16404344693699999</v>
+        <v>0.141882067409</v>
       </c>
       <c r="N41" s="1">
-        <v>-0.10459503367</v>
+        <v>3.7891371477800001E-2</v>
       </c>
       <c r="O41" s="1">
-        <v>4.14883552532E-2</v>
+        <v>4.7833759067999998E-2</v>
       </c>
       <c r="P41" s="1">
-        <v>0.148832811812</v>
+        <v>0.10641215232200001</v>
       </c>
       <c r="Q41" s="1">
-        <v>0.231808480634</v>
+        <v>0.27920346198599999</v>
       </c>
       <c r="R41" s="1">
-        <v>0.23560452302599999</v>
+        <v>0.31881210916399999</v>
       </c>
       <c r="S41" s="1">
-        <v>0.39562730392399997</v>
+        <v>0.32153007002400003</v>
       </c>
       <c r="T41" s="1">
-        <v>0.34246174276199998</v>
+        <v>0.29541794354599998</v>
       </c>
       <c r="U41" s="1">
-        <v>0.18386749916799999</v>
+        <v>0.30436468460299998</v>
       </c>
       <c r="V41" s="1">
-        <v>0.20790478054100001</v>
+        <v>0.16602843689399999</v>
       </c>
       <c r="W41" s="1">
-        <v>0.197614419012</v>
+        <v>0.140634922202</v>
       </c>
       <c r="X41" s="1">
-        <v>0.21458733369300001</v>
+        <v>0.26291910826300002</v>
       </c>
       <c r="Y41" s="1">
-        <v>0.12575299671000001</v>
+        <v>0.22612603824700001</v>
       </c>
       <c r="Z41" s="1">
-        <v>0.49509766183800002</v>
+        <v>0.45380355293000002</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B42" s="1">
-        <v>-4.6362763452400001E-2</v>
+        <v>-3.5817667495400003E-2</v>
       </c>
       <c r="C42" s="1">
-        <v>9.1678388138100003E-2</v>
+        <v>9.1584697625299999E-2</v>
       </c>
       <c r="D42" s="1">
-        <v>-0.14665480549500001</v>
+        <v>2.09327344025E-2</v>
       </c>
       <c r="E42" s="1">
-        <v>5.2660642245500003E-2</v>
+        <v>6.1858432602200003E-2</v>
       </c>
       <c r="F42" s="1">
-        <v>0.121185620085</v>
+        <v>4.7959149726899998E-2</v>
       </c>
       <c r="G42" s="1">
-        <v>-0.13983768101499999</v>
+        <v>-3.2953119695799997E-2</v>
       </c>
       <c r="H42" s="1">
-        <v>0.24253301530800001</v>
+        <v>0.161962734783</v>
       </c>
       <c r="I42" s="1">
-        <v>-0.255244460058</v>
+        <v>8.0787710002399996E-4</v>
       </c>
       <c r="J42" s="1">
-        <v>1.2710034749500001E-3</v>
+        <v>6.6172815304599994E-2</v>
       </c>
       <c r="K42" s="1">
-        <v>0.20935788267200001</v>
+        <v>7.6294283020599998E-2</v>
       </c>
       <c r="L42" s="1">
-        <v>-0.13196519151</v>
+        <v>-3.9443477882199998E-2</v>
       </c>
       <c r="M42" s="1">
-        <v>0.232490737945</v>
+        <v>0.165228532613</v>
       </c>
       <c r="N42" s="1">
-        <v>-0.26056082015900001</v>
+        <v>7.7846250252499999E-3</v>
       </c>
       <c r="O42" s="1">
-        <v>1.77899341702E-2</v>
+        <v>7.5836054328800001E-2</v>
       </c>
       <c r="P42" s="1">
-        <v>0.21400803189000001</v>
+        <v>7.9448567880199994E-2</v>
       </c>
       <c r="Q42" s="1">
-        <v>0.18665646704</v>
+        <v>0.36031233327700002</v>
       </c>
       <c r="R42" s="1">
-        <v>0.26202315465199999</v>
+        <v>0.43906338901899999</v>
       </c>
       <c r="S42" s="1">
-        <v>0.214212157938</v>
+        <v>0.427419992473</v>
       </c>
       <c r="T42" s="1">
-        <v>0.16601334752800001</v>
+        <v>0.41378428965199998</v>
       </c>
       <c r="U42" s="1">
-        <v>0.12084235552</v>
+        <v>0.39720121516200002</v>
       </c>
       <c r="V42" s="1">
-        <v>9.8716921218700002E-2</v>
+        <v>0.267081134346</v>
       </c>
       <c r="W42" s="1">
-        <v>0.169134016538</v>
+        <v>0.22497140585100001</v>
       </c>
       <c r="X42" s="1">
-        <v>0.11900167495400001</v>
+        <v>0.383650878902</v>
       </c>
       <c r="Y42" s="1">
-        <v>2.2421252900100001E-2</v>
+        <v>0.36304065129300001</v>
       </c>
       <c r="Z42" s="1">
-        <v>0.36078528477100003</v>
+        <v>0.51636992098800005</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B43" s="1">
-        <v>-5.0317598706999998E-2</v>
+        <v>-3.1189675450800002E-2</v>
       </c>
       <c r="C43" s="1">
-        <v>6.2933488684199998E-2</v>
+        <v>4.86474404919E-2</v>
       </c>
       <c r="D43" s="1">
-        <v>-0.14791036896199999</v>
+        <v>-2.5296086075100001E-2</v>
       </c>
       <c r="E43" s="1">
-        <v>3.9501523011600002E-2</v>
+        <v>9.2075988445800006E-2</v>
       </c>
       <c r="F43" s="1">
-        <v>0.126412989783</v>
+        <v>5.3935724810800001E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>-0.10416190784899999</v>
+        <v>-8.2157628113399994E-2</v>
       </c>
       <c r="H43" s="1">
-        <v>0.170087553823</v>
+        <v>0.152722669374</v>
       </c>
       <c r="I43" s="1">
-        <v>-0.18164769329899999</v>
+        <v>4.34554878329E-2</v>
       </c>
       <c r="J43" s="1">
-        <v>3.7980983155299998E-2</v>
+        <v>2.3217635633599999E-2</v>
       </c>
       <c r="K43" s="1">
-        <v>0.176411075463</v>
+        <v>6.5830212838800001E-2</v>
       </c>
       <c r="L43" s="1">
-        <v>-0.100479599216</v>
+        <v>-7.9110748520499999E-2</v>
       </c>
       <c r="M43" s="1">
-        <v>0.158267583346</v>
+        <v>0.144250769433</v>
       </c>
       <c r="N43" s="1">
-        <v>-0.193620444966</v>
+        <v>2.9309367954899999E-2</v>
       </c>
       <c r="O43" s="1">
-        <v>4.3051228816999999E-2</v>
+        <v>4.7280732657299998E-2</v>
       </c>
       <c r="P43" s="1">
-        <v>0.18277846148400001</v>
+        <v>7.1997185376900003E-2</v>
       </c>
       <c r="Q43" s="1">
-        <v>0.13858605153600001</v>
+        <v>0.38642427277500002</v>
       </c>
       <c r="R43" s="1">
-        <v>0.156678341226</v>
+        <v>0.47355002546800001</v>
       </c>
       <c r="S43" s="1">
-        <v>0.168963023144</v>
+        <v>0.38699418011600001</v>
       </c>
       <c r="T43" s="1">
-        <v>0.130971095368</v>
+        <v>0.35952585422900002</v>
       </c>
       <c r="U43" s="1">
-        <v>0.11836752268</v>
+        <v>0.425600802705</v>
       </c>
       <c r="V43" s="1">
-        <v>0.105679128469</v>
+        <v>0.24453599614400001</v>
       </c>
       <c r="W43" s="1">
-        <v>0.111552146031</v>
+        <v>0.228946401524</v>
       </c>
       <c r="X43" s="1">
-        <v>0.12158260683</v>
+        <v>0.32333439885199999</v>
       </c>
       <c r="Y43" s="1">
-        <v>-2.58537155045E-2</v>
+        <v>0.34610292920899999</v>
       </c>
       <c r="Z43" s="1">
-        <v>0.35006815432900001</v>
+        <v>0.45625767749099999</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B44" s="1">
-        <v>-3.7813053008699998E-2</v>
+        <v>1.7690629764599999E-3</v>
       </c>
       <c r="C44" s="1">
-        <v>9.7681366783599996E-2</v>
+        <v>5.1348427399600001E-2</v>
       </c>
       <c r="D44" s="1">
-        <v>-7.9157589987099999E-2</v>
+        <v>2.5125257576199999E-2</v>
       </c>
       <c r="E44" s="1">
-        <v>7.7245938801999994E-2</v>
+        <v>4.7752578873299999E-2</v>
       </c>
       <c r="F44" s="1">
-        <v>9.3039134756700004E-2</v>
+        <v>7.36955385543E-2</v>
       </c>
       <c r="G44" s="1">
-        <v>-9.6200206600900007E-2</v>
+        <v>-5.5882109569099997E-3</v>
       </c>
       <c r="H44" s="1">
-        <v>0.19726526125800001</v>
+        <v>9.6245854573600007E-2</v>
       </c>
       <c r="I44" s="1">
-        <v>-0.17023596491199999</v>
+        <v>4.5379994655500001E-2</v>
       </c>
       <c r="J44" s="1">
-        <v>3.2165474704699999E-2</v>
+        <v>6.4317832916699999E-2</v>
       </c>
       <c r="K44" s="1">
-        <v>0.15504665208499999</v>
+        <v>0.107470280694</v>
       </c>
       <c r="L44" s="1">
-        <v>-9.36146199245E-2</v>
+        <v>-4.0366512223999999E-3</v>
       </c>
       <c r="M44" s="1">
-        <v>0.19877431251399999</v>
+        <v>9.4908058614099997E-2</v>
       </c>
       <c r="N44" s="1">
-        <v>-0.16981258885</v>
+        <v>4.5051907139499997E-2</v>
       </c>
       <c r="O44" s="1">
-        <v>5.3065523246200001E-2</v>
+        <v>6.7630911737000005E-2</v>
       </c>
       <c r="P44" s="1">
-        <v>0.161727526958</v>
+        <v>0.111105518518</v>
       </c>
       <c r="Q44" s="1">
-        <v>0.175028240197</v>
+        <v>0.31949992458900001</v>
       </c>
       <c r="R44" s="1">
-        <v>0.137746853192</v>
+        <v>0.44303051447500003</v>
       </c>
       <c r="S44" s="1">
-        <v>0.213329747771</v>
+        <v>0.34813304121100003</v>
       </c>
       <c r="T44" s="1">
-        <v>0.18739182988399999</v>
+        <v>0.31137035045400002</v>
       </c>
       <c r="U44" s="1">
-        <v>7.9642384087699997E-2</v>
+        <v>0.394806687928</v>
       </c>
       <c r="V44" s="1">
-        <v>0.138809134004</v>
+        <v>0.203568968578</v>
       </c>
       <c r="W44" s="1">
-        <v>0.146353947983</v>
+        <v>0.21532745219900001</v>
       </c>
       <c r="X44" s="1">
-        <v>0.105778131044</v>
+        <v>0.37168828921699998</v>
       </c>
       <c r="Y44" s="1">
-        <v>-3.5151933079199997E-2</v>
+        <v>0.34070829022400001</v>
       </c>
       <c r="Z44" s="1">
-        <v>0.30549079383700001</v>
+        <v>0.473039622351</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="B45" s="1">
-        <v>-0.209051073601</v>
+        <v>-4.9356262117300001E-2</v>
       </c>
       <c r="C45" s="1">
-        <v>0.77097017273400004</v>
+        <v>7.3860828859200006E-2</v>
       </c>
       <c r="D45" s="1">
-        <v>-0.28482687326</v>
+        <v>2.9052145772599999E-2</v>
       </c>
       <c r="E45" s="1">
-        <v>-0.25037132415800001</v>
+        <v>9.2867531534299996E-2</v>
       </c>
       <c r="F45" s="1">
-        <v>0.50660248562999999</v>
+        <v>6.4420701104699996E-2</v>
       </c>
       <c r="G45" s="1">
-        <v>-9.1662349487699996E-2</v>
+        <v>-2.4376765478399998E-2</v>
       </c>
       <c r="H45" s="1">
-        <v>0.232995933618</v>
+        <v>0.121442021668</v>
       </c>
       <c r="I45" s="1">
-        <v>-6.3257908857600006E-2</v>
+        <v>8.3759628983599996E-2</v>
       </c>
       <c r="J45" s="1">
-        <v>-2.63961174231E-2</v>
+        <v>8.1917605886699996E-2</v>
       </c>
       <c r="K45" s="1">
-        <v>-2.49418048305E-2</v>
+        <v>0.121121554258</v>
       </c>
       <c r="L45" s="1">
-        <v>-0.13822513591999999</v>
+        <v>-3.6884993195999999E-2</v>
       </c>
       <c r="M45" s="1">
-        <v>0.41430255681700001</v>
+        <v>0.12536203219100001</v>
       </c>
       <c r="N45" s="1">
-        <v>-0.132159722782</v>
+        <v>7.9036392638200004E-2</v>
       </c>
       <c r="O45" s="1">
-        <v>-8.95873794453E-2</v>
+        <v>9.9215506699999997E-2</v>
       </c>
       <c r="P45" s="1">
-        <v>0.10979977150299999</v>
+        <v>0.121935047724</v>
       </c>
       <c r="Q45" s="1">
-        <v>-4.38867109958E-2</v>
+        <v>0.372122777628</v>
       </c>
       <c r="R45" s="1">
-        <v>0.58822227428200002</v>
+        <v>0.47004949580900002</v>
       </c>
       <c r="S45" s="1">
-        <v>-5.4156821288300003E-2</v>
+        <v>0.42363550668</v>
       </c>
       <c r="T45" s="1">
-        <v>3.1962119058200002E-3</v>
+        <v>0.40569293974300003</v>
       </c>
       <c r="U45" s="1">
-        <v>2.48294967683E-3</v>
+        <v>0.39750788179000002</v>
       </c>
       <c r="V45" s="1">
-        <v>-0.38289976702200001</v>
+        <v>0.24354709608700001</v>
       </c>
       <c r="W45" s="1">
-        <v>0.59194758621599997</v>
+        <v>0.240934412376</v>
       </c>
       <c r="X45" s="1">
-        <v>-0.30571551098100003</v>
+        <v>0.38180046187299999</v>
       </c>
       <c r="Y45" s="1">
-        <v>-0.47826164498399998</v>
+        <v>0.37819101847199998</v>
       </c>
       <c r="Z45" s="1">
-        <v>4.6080798126099998E-2</v>
+        <v>0.55175710154099999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>